<commit_message>
Removed project name from the template
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/WATR_Template.xlsx
+++ b/AxeAccessibilityDriver/WATR_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27462375-23DB-4259-8E6B-ADF44FD62D28}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC3B87A-F246-4E46-BC6B-15CC981A210D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="253">
   <si>
     <t>1.1.1</t>
   </si>
@@ -2353,12 +2353,6 @@
   </si>
   <si>
     <t>Progress to 100% Compliance</t>
-  </si>
-  <si>
-    <t>CGRT Cognos Analytics Accessibility Report</t>
-  </si>
-  <si>
-    <t>Levon Minasyan, Aarzoo Chennan, Jing Zhang</t>
   </si>
   <si>
     <t>Attaching list of pages that is covered by AODA testing in Cognos application. Also including Closed and Outstanding defects lists below.</t>
@@ -3709,6 +3703,9 @@
     <xf numFmtId="168" fontId="29" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3872,9 +3869,6 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -5227,8 +5221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AF9770-A07B-4681-91C3-E6CA1B6C7937}">
   <dimension ref="A1:IR30"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5534,9 +5528,7 @@
       <c r="IR3" s="121"/>
     </row>
     <row r="4" spans="1:252" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
-        <v>243</v>
-      </c>
+      <c r="A4" s="81"/>
       <c r="B4" s="46"/>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
@@ -5815,9 +5807,7 @@
       <c r="IR6" s="121"/>
     </row>
     <row r="7" spans="1:252" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="81" t="s">
-        <v>244</v>
-      </c>
+      <c r="A7" s="81"/>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
       <c r="D7" s="46"/>
@@ -6097,7 +6087,7 @@
     </row>
     <row r="10" spans="1:252" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="81" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B10" s="46"/>
       <c r="C10" s="46"/>
@@ -6378,7 +6368,7 @@
     </row>
     <row r="13" spans="1:252" ht="366.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="81" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B13" s="46"/>
       <c r="C13" s="46"/>
@@ -6659,7 +6649,7 @@
     </row>
     <row r="16" spans="1:252" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="81" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B16" s="46"/>
       <c r="C16" s="46"/>
@@ -6697,7 +6687,7 @@
     </row>
     <row r="19" spans="1:9" ht="348" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="81" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="42"/>
@@ -6722,7 +6712,7 @@
     </row>
     <row r="21" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="81" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6732,12 +6722,12 @@
     </row>
     <row r="23" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="81" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="124" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6784,7 +6774,7 @@
   </sheetPr>
   <dimension ref="A1:XFC81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -6810,16 +6800,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="187" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
-      <c r="G1" s="186"/>
-      <c r="H1" s="187"/>
+      <c r="B1" s="187"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="188"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
@@ -6833,13 +6823,13 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="168" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="191"/>
+      <c r="B2" s="168"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="192"/>
       <c r="F2" s="30"/>
       <c r="G2" s="1"/>
       <c r="H2" s="7"/>
@@ -6851,13 +6841,13 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="167" t="s">
+      <c r="A3" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="167"/>
-      <c r="C3" s="203"/>
-      <c r="D3" s="204"/>
-      <c r="E3" s="205"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="205"/>
+      <c r="E3" s="206"/>
       <c r="F3" s="30"/>
       <c r="G3" s="1"/>
       <c r="H3" s="7"/>
@@ -6869,12 +6859,12 @@
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="167" t="s">
+      <c r="A4" s="168" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="167"/>
-      <c r="C4" s="213"/>
-      <c r="D4" s="213"/>
+      <c r="B4" s="168"/>
+      <c r="C4" s="214"/>
+      <c r="D4" s="214"/>
       <c r="E4" s="82"/>
       <c r="F4" s="30"/>
       <c r="G4" s="1"/>
@@ -6887,13 +6877,13 @@
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="166" t="s">
+      <c r="A5" s="167" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="166"/>
-      <c r="C5" s="214"/>
-      <c r="D5" s="214"/>
-      <c r="E5" s="215"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="215"/>
+      <c r="D5" s="215"/>
+      <c r="E5" s="216"/>
       <c r="F5" s="30"/>
       <c r="G5" s="1"/>
       <c r="H5" s="7"/>
@@ -6905,13 +6895,13 @@
       <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="166" t="s">
+      <c r="A6" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="166"/>
-      <c r="C6" s="164"/>
-      <c r="D6" s="164"/>
-      <c r="E6" s="165"/>
+      <c r="B6" s="167"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="166"/>
       <c r="F6" s="30"/>
       <c r="G6" s="1"/>
       <c r="H6" s="7"/>
@@ -6923,13 +6913,13 @@
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="166" t="s">
+      <c r="A7" s="167" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="166"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="164"/>
-      <c r="E7" s="165"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="166"/>
       <c r="F7" s="30"/>
       <c r="G7" s="1"/>
       <c r="H7" s="7"/>
@@ -6941,13 +6931,13 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="166" t="s">
+      <c r="A8" s="167" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="166"/>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="165"/>
+      <c r="B8" s="167"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="166"/>
       <c r="F8" s="30"/>
       <c r="G8" s="1"/>
       <c r="H8" s="7"/>
@@ -6959,16 +6949,16 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:19" s="28" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="194" t="s">
+      <c r="A9" s="195" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="195"/>
-      <c r="C9" s="195"/>
-      <c r="D9" s="195"/>
-      <c r="E9" s="195"/>
-      <c r="F9" s="195"/>
-      <c r="G9" s="195"/>
-      <c r="H9" s="195"/>
+      <c r="B9" s="196"/>
+      <c r="C9" s="196"/>
+      <c r="D9" s="196"/>
+      <c r="E9" s="196"/>
+      <c r="F9" s="196"/>
+      <c r="G9" s="196"/>
+      <c r="H9" s="196"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -6978,16 +6968,16 @@
       <c r="Q9" s="99"/>
     </row>
     <row r="10" spans="1:19" s="13" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="196" t="s">
+      <c r="A10" s="197" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="197"/>
-      <c r="C10" s="197"/>
-      <c r="D10" s="197"/>
-      <c r="E10" s="197"/>
-      <c r="F10" s="197"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="198"/>
+      <c r="B10" s="198"/>
+      <c r="C10" s="198"/>
+      <c r="D10" s="198"/>
+      <c r="E10" s="198"/>
+      <c r="F10" s="198"/>
+      <c r="G10" s="198"/>
+      <c r="H10" s="199"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -6997,10 +6987,10 @@
       <c r="Q10" s="14"/>
     </row>
     <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="201" t="s">
+      <c r="A11" s="202" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="202"/>
+      <c r="B11" s="203"/>
       <c r="C11" s="105" t="s">
         <v>40</v>
       </c>
@@ -7010,10 +7000,10 @@
       <c r="E11" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="200" t="s">
+      <c r="F11" s="201" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="200"/>
+      <c r="G11" s="201"/>
       <c r="H11" s="106" t="s">
         <v>53</v>
       </c>
@@ -7025,18 +7015,18 @@
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="192" t="s">
+      <c r="A12" s="193" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="193"/>
-      <c r="C12" s="183" t="s">
+      <c r="B12" s="194"/>
+      <c r="C12" s="184" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="185"/>
+      <c r="D12" s="185"/>
+      <c r="E12" s="185"/>
+      <c r="F12" s="185"/>
+      <c r="G12" s="185"/>
+      <c r="H12" s="186"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -7052,12 +7042,12 @@
         <v>41</v>
       </c>
       <c r="C13" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D13" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="218"/>
+      <c r="E13" s="162"/>
       <c r="F13" s="88">
         <f>IF(D13="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7083,12 +7073,12 @@
         <v>42</v>
       </c>
       <c r="C14" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D14" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="218"/>
+      <c r="E14" s="162"/>
       <c r="F14" s="88">
         <f>IF(D14="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7114,12 +7104,12 @@
         <v>152</v>
       </c>
       <c r="C15" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D15" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="218"/>
+      <c r="E15" s="162"/>
       <c r="F15" s="88">
         <f t="shared" ref="F15:F26" si="1">IF(D15="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7145,12 +7135,12 @@
         <v>43</v>
       </c>
       <c r="C16" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D16" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="218"/>
+      <c r="E16" s="162"/>
       <c r="F16" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7176,12 +7166,12 @@
         <v>44</v>
       </c>
       <c r="C17" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D17" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="218"/>
+      <c r="E17" s="162"/>
       <c r="F17" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7207,12 +7197,12 @@
         <v>45</v>
       </c>
       <c r="C18" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D18" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="218"/>
+      <c r="E18" s="162"/>
       <c r="F18" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7238,12 +7228,12 @@
         <v>224</v>
       </c>
       <c r="C19" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D19" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="218"/>
+      <c r="E19" s="162"/>
       <c r="F19" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7271,12 +7261,12 @@
         <v>180</v>
       </c>
       <c r="C20" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D20" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="218"/>
+      <c r="E20" s="162"/>
       <c r="F20" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7304,12 +7294,12 @@
         <v>181</v>
       </c>
       <c r="C21" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D21" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="218"/>
+      <c r="E21" s="162"/>
       <c r="F21" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7337,12 +7327,12 @@
         <v>46</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D22" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="218"/>
+      <c r="E22" s="162"/>
       <c r="F22" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7370,12 +7360,12 @@
         <v>201</v>
       </c>
       <c r="C23" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D23" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="218"/>
+      <c r="E23" s="162"/>
       <c r="F23" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7401,12 +7391,12 @@
         <v>182</v>
       </c>
       <c r="C24" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D24" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="218"/>
+      <c r="E24" s="162"/>
       <c r="F24" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7434,12 +7424,12 @@
         <v>183</v>
       </c>
       <c r="C25" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D25" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="218"/>
+      <c r="E25" s="162"/>
       <c r="F25" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7465,12 +7455,12 @@
         <v>184</v>
       </c>
       <c r="C26" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D26" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="218"/>
+      <c r="E26" s="162"/>
       <c r="F26" s="88">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7489,14 +7479,14 @@
       <c r="Q26" s="93"/>
     </row>
     <row r="27" spans="1:17" ht="17.45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="188" t="s">
+      <c r="A27" s="189" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="189"/>
-      <c r="C27" s="189"/>
-      <c r="D27" s="189"/>
-      <c r="E27" s="189"/>
-      <c r="F27" s="189"/>
+      <c r="B27" s="190"/>
+      <c r="C27" s="190"/>
+      <c r="D27" s="190"/>
+      <c r="E27" s="190"/>
+      <c r="F27" s="190"/>
       <c r="G27" s="15">
         <f>SUM(H13:H26)</f>
         <v>0</v>
@@ -7513,18 +7503,18 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="192" t="s">
+      <c r="A28" s="193" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="199"/>
-      <c r="C28" s="183" t="s">
+      <c r="B28" s="200"/>
+      <c r="C28" s="184" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="184"/>
-      <c r="E28" s="184"/>
-      <c r="F28" s="184"/>
-      <c r="G28" s="184"/>
-      <c r="H28" s="185"/>
+      <c r="D28" s="185"/>
+      <c r="E28" s="185"/>
+      <c r="F28" s="185"/>
+      <c r="G28" s="185"/>
+      <c r="H28" s="186"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -7540,12 +7530,12 @@
         <v>47</v>
       </c>
       <c r="C29" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D29" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="218"/>
+      <c r="E29" s="162"/>
       <c r="F29" s="88">
         <f t="shared" ref="F29:F40" si="2">IF(D29="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7571,12 +7561,12 @@
         <v>202</v>
       </c>
       <c r="C30" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D30" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="218"/>
+      <c r="E30" s="162"/>
       <c r="F30" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7602,12 +7592,12 @@
         <v>62</v>
       </c>
       <c r="C31" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D31" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="218"/>
+      <c r="E31" s="162"/>
       <c r="F31" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7633,12 +7623,12 @@
         <v>203</v>
       </c>
       <c r="C32" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D32" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E32" s="218"/>
+      <c r="E32" s="162"/>
       <c r="F32" s="88"/>
       <c r="G32" s="89"/>
       <c r="H32" s="90">
@@ -7661,12 +7651,12 @@
         <v>186</v>
       </c>
       <c r="C33" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D33" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E33" s="218"/>
+      <c r="E33" s="162"/>
       <c r="F33" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7692,12 +7682,12 @@
         <v>187</v>
       </c>
       <c r="C34" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D34" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="218"/>
+      <c r="E34" s="162"/>
       <c r="F34" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7723,12 +7713,12 @@
         <v>204</v>
       </c>
       <c r="C35" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D35" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E35" s="218"/>
+      <c r="E35" s="162"/>
       <c r="F35" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7754,12 +7744,12 @@
         <v>188</v>
       </c>
       <c r="C36" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D36" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="218"/>
+      <c r="E36" s="162"/>
       <c r="F36" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7785,12 +7775,12 @@
         <v>48</v>
       </c>
       <c r="C37" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D37" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E37" s="218"/>
+      <c r="E37" s="162"/>
       <c r="F37" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7816,12 +7806,12 @@
         <v>189</v>
       </c>
       <c r="C38" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D38" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="218"/>
+      <c r="E38" s="162"/>
       <c r="F38" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7847,12 +7837,12 @@
         <v>205</v>
       </c>
       <c r="C39" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D39" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="218"/>
+      <c r="E39" s="162"/>
       <c r="F39" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7878,12 +7868,12 @@
         <v>49</v>
       </c>
       <c r="C40" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D40" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="218"/>
+      <c r="E40" s="162"/>
       <c r="F40" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7902,14 +7892,14 @@
       <c r="Q40" s="93"/>
     </row>
     <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="188" t="s">
+      <c r="A41" s="189" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="189"/>
-      <c r="C41" s="189"/>
-      <c r="D41" s="189"/>
-      <c r="E41" s="189"/>
-      <c r="F41" s="189"/>
+      <c r="B41" s="190"/>
+      <c r="C41" s="190"/>
+      <c r="D41" s="190"/>
+      <c r="E41" s="190"/>
+      <c r="F41" s="190"/>
       <c r="G41" s="15">
         <f>SUM(H29:H40)</f>
         <v>0</v>
@@ -7926,18 +7916,18 @@
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="192" t="s">
+      <c r="A42" s="193" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="199"/>
-      <c r="C42" s="183" t="s">
+      <c r="B42" s="200"/>
+      <c r="C42" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="184"/>
-      <c r="E42" s="184"/>
-      <c r="F42" s="184"/>
-      <c r="G42" s="184"/>
-      <c r="H42" s="185"/>
+      <c r="D42" s="185"/>
+      <c r="E42" s="185"/>
+      <c r="F42" s="185"/>
+      <c r="G42" s="185"/>
+      <c r="H42" s="186"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -7953,12 +7943,12 @@
         <v>191</v>
       </c>
       <c r="C43" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D43" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="218"/>
+      <c r="E43" s="162"/>
       <c r="F43" s="88">
         <f t="shared" ref="F43:F56" si="4">IF(D43="does not support","list date full support planned, if any &gt;",0)</f>
         <v>0</v>
@@ -7984,12 +7974,12 @@
         <v>38</v>
       </c>
       <c r="C44" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D44" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="218"/>
+      <c r="E44" s="162"/>
       <c r="F44" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8015,12 +8005,12 @@
         <v>206</v>
       </c>
       <c r="C45" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D45" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="218"/>
+      <c r="E45" s="162"/>
       <c r="F45" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8046,12 +8036,12 @@
         <v>192</v>
       </c>
       <c r="C46" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D46" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E46" s="218"/>
+      <c r="E46" s="162"/>
       <c r="F46" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8077,12 +8067,12 @@
         <v>193</v>
       </c>
       <c r="C47" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D47" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E47" s="218"/>
+      <c r="E47" s="162"/>
       <c r="F47" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8108,12 +8098,12 @@
         <v>194</v>
       </c>
       <c r="C48" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D48" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E48" s="218"/>
+      <c r="E48" s="162"/>
       <c r="F48" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8139,12 +8129,12 @@
         <v>207</v>
       </c>
       <c r="C49" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D49" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="218"/>
+      <c r="E49" s="162"/>
       <c r="F49" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8170,12 +8160,12 @@
         <v>208</v>
       </c>
       <c r="C50" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D50" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E50" s="218"/>
+      <c r="E50" s="162"/>
       <c r="F50" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8201,12 +8191,12 @@
         <v>209</v>
       </c>
       <c r="C51" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D51" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E51" s="218"/>
+      <c r="E51" s="162"/>
       <c r="F51" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8232,12 +8222,12 @@
         <v>195</v>
       </c>
       <c r="C52" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D52" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E52" s="218"/>
+      <c r="E52" s="162"/>
       <c r="F52" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8256,14 +8246,14 @@
       <c r="Q52" s="93"/>
     </row>
     <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="188" t="s">
+      <c r="A53" s="189" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="189"/>
-      <c r="C53" s="189"/>
-      <c r="D53" s="189"/>
-      <c r="E53" s="189"/>
-      <c r="F53" s="189"/>
+      <c r="B53" s="190"/>
+      <c r="C53" s="190"/>
+      <c r="D53" s="190"/>
+      <c r="E53" s="190"/>
+      <c r="F53" s="190"/>
       <c r="G53" s="16">
         <f>SUM(H43:H52)</f>
         <v>0</v>
@@ -8280,18 +8270,18 @@
       <c r="N53" s="4"/>
     </row>
     <row r="54" spans="1:17" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="209" t="s">
+      <c r="A54" s="210" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="210"/>
-      <c r="C54" s="206" t="s">
+      <c r="B54" s="211"/>
+      <c r="C54" s="207" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="207"/>
-      <c r="E54" s="207"/>
-      <c r="F54" s="207"/>
-      <c r="G54" s="207"/>
-      <c r="H54" s="208"/>
+      <c r="D54" s="208"/>
+      <c r="E54" s="208"/>
+      <c r="F54" s="208"/>
+      <c r="G54" s="208"/>
+      <c r="H54" s="209"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -8307,12 +8297,12 @@
         <v>50</v>
       </c>
       <c r="C55" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D55" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E55" s="218"/>
+      <c r="E55" s="162"/>
       <c r="F55" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8338,12 +8328,12 @@
         <v>51</v>
       </c>
       <c r="C56" s="85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D56" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="E56" s="218"/>
+      <c r="E56" s="162"/>
       <c r="F56" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8362,14 +8352,14 @@
       <c r="Q56" s="93"/>
     </row>
     <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="188" t="s">
+      <c r="A57" s="189" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="189"/>
-      <c r="C57" s="189"/>
-      <c r="D57" s="189"/>
-      <c r="E57" s="189"/>
-      <c r="F57" s="189"/>
+      <c r="B57" s="190"/>
+      <c r="C57" s="190"/>
+      <c r="D57" s="190"/>
+      <c r="E57" s="190"/>
+      <c r="F57" s="190"/>
       <c r="G57" s="15">
         <f>SUM(H55:H56)</f>
         <v>0</v>
@@ -8386,16 +8376,16 @@
       <c r="N57" s="4"/>
     </row>
     <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="211" t="s">
+      <c r="A58" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="212"/>
-      <c r="C58" s="212"/>
-      <c r="D58" s="212"/>
-      <c r="E58" s="212"/>
-      <c r="F58" s="180"/>
-      <c r="G58" s="181"/>
-      <c r="H58" s="182"/>
+      <c r="B58" s="213"/>
+      <c r="C58" s="213"/>
+      <c r="D58" s="213"/>
+      <c r="E58" s="213"/>
+      <c r="F58" s="181"/>
+      <c r="G58" s="182"/>
+      <c r="H58" s="183"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -8404,14 +8394,14 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="170"/>
-      <c r="B59" s="171"/>
+      <c r="A59" s="171"/>
+      <c r="B59" s="172"/>
       <c r="C59" s="19"/>
-      <c r="D59" s="177" t="s">
+      <c r="D59" s="178" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="178"/>
-      <c r="F59" s="179"/>
+      <c r="E59" s="179"/>
+      <c r="F59" s="180"/>
       <c r="G59" s="20">
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
@@ -8425,13 +8415,13 @@
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="172"/>
-      <c r="B60" s="173"/>
+      <c r="A60" s="173"/>
+      <c r="B60" s="174"/>
       <c r="C60" s="22"/>
-      <c r="D60" s="174" t="s">
+      <c r="D60" s="175" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="175"/>
+      <c r="E60" s="176"/>
       <c r="F60" s="23"/>
       <c r="G60" s="24"/>
       <c r="H60" s="25"/>
@@ -8443,13 +8433,13 @@
       <c r="N60" s="4"/>
     </row>
     <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="172"/>
-      <c r="B61" s="173"/>
+      <c r="A61" s="173"/>
+      <c r="B61" s="174"/>
       <c r="C61" s="22"/>
-      <c r="D61" s="174" t="s">
+      <c r="D61" s="175" t="s">
         <v>56</v>
       </c>
-      <c r="E61" s="175"/>
+      <c r="E61" s="176"/>
       <c r="F61" s="23"/>
       <c r="G61" s="24"/>
       <c r="H61" s="25"/>
@@ -8461,13 +8451,13 @@
       <c r="N61" s="4"/>
     </row>
     <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="172"/>
-      <c r="B62" s="173"/>
+      <c r="A62" s="173"/>
+      <c r="B62" s="174"/>
       <c r="C62" s="26"/>
-      <c r="D62" s="176" t="s">
+      <c r="D62" s="177" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="175"/>
+      <c r="E62" s="176"/>
       <c r="F62" s="23"/>
       <c r="G62" s="24"/>
       <c r="H62" s="25"/>
@@ -8486,11 +8476,11 @@
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="168" t="s">
+      <c r="E63" s="169" t="s">
         <v>154</v>
       </c>
-      <c r="F63" s="168"/>
-      <c r="G63" s="169"/>
+      <c r="F63" s="169"/>
+      <c r="G63" s="170"/>
       <c r="H63" s="34"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -8500,10 +8490,10 @@
       <c r="N63" s="4"/>
     </row>
     <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="162" t="s">
+      <c r="A64" s="163" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="163"/>
+      <c r="B64" s="164"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
       <c r="E64" s="35"/>
@@ -9129,16 +9119,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="130" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="217" t="s">
+      <c r="A1" s="218" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="217"/>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="217"/>
-      <c r="H1" s="217"/>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
       <c r="I1" s="128"/>
       <c r="J1" s="128"/>
       <c r="K1" s="128"/>
@@ -9150,16 +9140,16 @@
       <c r="Q1" s="129"/>
     </row>
     <row r="2" spans="1:20" s="135" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="216" t="s">
+      <c r="A2" s="217" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="216"/>
-      <c r="C2" s="216"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
-      <c r="G2" s="216"/>
-      <c r="H2" s="216"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="217"/>
       <c r="I2" s="131"/>
       <c r="J2" s="132"/>
       <c r="K2" s="132"/>
@@ -9230,7 +9220,7 @@
       <c r="G5" s="151"/>
       <c r="H5" s="144"/>
       <c r="L5" s="152" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="M5" s="146" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Broken link to updates on the template
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/WATR_Template.xlsx
+++ b/AxeAccessibilityDriver/WATR_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932ACAF4-B1FE-4103-9EC8-42AEF8279246}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31067212-021C-4A5D-88F4-B9B9F6073F2D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -3669,22 +3669,121 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="13" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3727,105 +3826,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4675,7 +4675,7 @@
   <cols>
     <col min="1" max="1" width="153.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="50" hidden="1" customWidth="1"/>
-    <col min="3" max="7" width="8.85546875" style="50" hidden="1"/>
+    <col min="3" max="7" width="8.85546875" style="50" hidden="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -5221,7 +5221,6 @@
         <v>61</v>
       </c>
       <c r="B2" s="48" t="e">
-        <f>COUNTIF('[3]WCAG 2.0 Compliance Checklist'!D13:D56,"Pass")</f>
         <v>#VALUE!</v>
       </c>
       <c r="C2" s="42"/>
@@ -5236,7 +5235,6 @@
         <v>94</v>
       </c>
       <c r="B3" s="44" t="e">
-        <f>COUNTIF('[3]WCAG 2.0 Compliance Checklist'!D13:D56,"Criteria not applicable")</f>
         <v>#VALUE!</v>
       </c>
       <c r="C3" s="44"/>
@@ -6755,16 +6753,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="180" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-      <c r="H1" s="188"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="181"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
@@ -6778,13 +6776,13 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="182" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="168"/>
-      <c r="C2" s="191"/>
-      <c r="D2" s="191"/>
-      <c r="E2" s="192"/>
+      <c r="B2" s="182"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="184"/>
       <c r="F2" s="30"/>
       <c r="G2" s="1"/>
       <c r="H2" s="7"/>
@@ -6796,13 +6794,13 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="182" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="168"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="205"/>
-      <c r="E3" s="206"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="199"/>
       <c r="F3" s="30"/>
       <c r="G3" s="1"/>
       <c r="H3" s="7"/>
@@ -6814,12 +6812,12 @@
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="168" t="s">
+      <c r="A4" s="182" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="168"/>
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
+      <c r="B4" s="182"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
       <c r="E4" s="82"/>
       <c r="F4" s="30"/>
       <c r="G4" s="1"/>
@@ -6832,13 +6830,13 @@
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="167" t="s">
+      <c r="A5" s="164" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="167"/>
-      <c r="C5" s="215"/>
-      <c r="D5" s="215"/>
-      <c r="E5" s="216"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="166"/>
       <c r="F5" s="30"/>
       <c r="G5" s="1"/>
       <c r="H5" s="7"/>
@@ -6850,13 +6848,13 @@
       <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="167" t="s">
+      <c r="A6" s="164" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="167"/>
-      <c r="C6" s="165"/>
-      <c r="D6" s="165"/>
-      <c r="E6" s="166"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
+      <c r="E6" s="168"/>
       <c r="F6" s="30"/>
       <c r="G6" s="1"/>
       <c r="H6" s="7"/>
@@ -6868,13 +6866,13 @@
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="167" t="s">
+      <c r="A7" s="164" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="167"/>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="166"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="167"/>
+      <c r="E7" s="168"/>
       <c r="F7" s="30"/>
       <c r="G7" s="1"/>
       <c r="H7" s="7"/>
@@ -6886,13 +6884,13 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="167" t="s">
+      <c r="A8" s="164" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="167"/>
-      <c r="C8" s="165"/>
-      <c r="D8" s="165"/>
-      <c r="E8" s="166"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="167"/>
+      <c r="D8" s="167"/>
+      <c r="E8" s="168"/>
       <c r="F8" s="30"/>
       <c r="G8" s="1"/>
       <c r="H8" s="7"/>
@@ -6904,16 +6902,16 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:19" s="28" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="195" t="s">
+      <c r="A9" s="186" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="196"/>
-      <c r="C9" s="196"/>
-      <c r="D9" s="196"/>
-      <c r="E9" s="196"/>
-      <c r="F9" s="196"/>
-      <c r="G9" s="196"/>
-      <c r="H9" s="196"/>
+      <c r="B9" s="187"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="187"/>
+      <c r="H9" s="187"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -6923,16 +6921,16 @@
       <c r="Q9" s="99"/>
     </row>
     <row r="10" spans="1:19" s="13" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="197" t="s">
+      <c r="A10" s="188" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="198"/>
-      <c r="C10" s="198"/>
-      <c r="D10" s="198"/>
-      <c r="E10" s="198"/>
-      <c r="F10" s="198"/>
-      <c r="G10" s="198"/>
-      <c r="H10" s="199"/>
+      <c r="B10" s="189"/>
+      <c r="C10" s="189"/>
+      <c r="D10" s="189"/>
+      <c r="E10" s="189"/>
+      <c r="F10" s="189"/>
+      <c r="G10" s="189"/>
+      <c r="H10" s="190"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -6942,10 +6940,10 @@
       <c r="Q10" s="14"/>
     </row>
     <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="202" t="s">
+      <c r="A11" s="195" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="203"/>
+      <c r="B11" s="196"/>
       <c r="C11" s="105" t="s">
         <v>40</v>
       </c>
@@ -6955,10 +6953,10 @@
       <c r="E11" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="201" t="s">
+      <c r="F11" s="191" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="201"/>
+      <c r="G11" s="191"/>
       <c r="H11" s="106" t="s">
         <v>53</v>
       </c>
@@ -6970,18 +6968,18 @@
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="193" t="s">
+      <c r="A12" s="174" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="194"/>
-      <c r="C12" s="184" t="s">
+      <c r="B12" s="185"/>
+      <c r="C12" s="192" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="185"/>
-      <c r="E12" s="185"/>
-      <c r="F12" s="185"/>
-      <c r="G12" s="185"/>
-      <c r="H12" s="186"/>
+      <c r="D12" s="193"/>
+      <c r="E12" s="193"/>
+      <c r="F12" s="193"/>
+      <c r="G12" s="193"/>
+      <c r="H12" s="194"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -7434,14 +7432,14 @@
       <c r="Q26" s="93"/>
     </row>
     <row r="27" spans="1:17" ht="17.45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="189" t="s">
+      <c r="A27" s="178" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="190"/>
-      <c r="C27" s="190"/>
-      <c r="D27" s="190"/>
-      <c r="E27" s="190"/>
-      <c r="F27" s="190"/>
+      <c r="B27" s="179"/>
+      <c r="C27" s="179"/>
+      <c r="D27" s="179"/>
+      <c r="E27" s="179"/>
+      <c r="F27" s="179"/>
       <c r="G27" s="15">
         <f>SUM(H13:H26)</f>
         <v>0</v>
@@ -7458,18 +7456,18 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="193" t="s">
+      <c r="A28" s="174" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="200"/>
-      <c r="C28" s="184" t="s">
+      <c r="B28" s="175"/>
+      <c r="C28" s="192" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="185"/>
-      <c r="E28" s="185"/>
-      <c r="F28" s="185"/>
-      <c r="G28" s="185"/>
-      <c r="H28" s="186"/>
+      <c r="D28" s="193"/>
+      <c r="E28" s="193"/>
+      <c r="F28" s="193"/>
+      <c r="G28" s="193"/>
+      <c r="H28" s="194"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -7847,14 +7845,14 @@
       <c r="Q40" s="93"/>
     </row>
     <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="189" t="s">
+      <c r="A41" s="178" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="190"/>
-      <c r="C41" s="190"/>
-      <c r="D41" s="190"/>
-      <c r="E41" s="190"/>
-      <c r="F41" s="190"/>
+      <c r="B41" s="179"/>
+      <c r="C41" s="179"/>
+      <c r="D41" s="179"/>
+      <c r="E41" s="179"/>
+      <c r="F41" s="179"/>
       <c r="G41" s="15">
         <f>SUM(H29:H40)</f>
         <v>0</v>
@@ -7871,18 +7869,18 @@
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="193" t="s">
+      <c r="A42" s="174" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="200"/>
-      <c r="C42" s="184" t="s">
+      <c r="B42" s="175"/>
+      <c r="C42" s="192" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="185"/>
-      <c r="E42" s="185"/>
-      <c r="F42" s="185"/>
-      <c r="G42" s="185"/>
-      <c r="H42" s="186"/>
+      <c r="D42" s="193"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="193"/>
+      <c r="G42" s="193"/>
+      <c r="H42" s="194"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -8201,14 +8199,14 @@
       <c r="Q52" s="93"/>
     </row>
     <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="189" t="s">
+      <c r="A53" s="178" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="190"/>
-      <c r="C53" s="190"/>
-      <c r="D53" s="190"/>
-      <c r="E53" s="190"/>
-      <c r="F53" s="190"/>
+      <c r="B53" s="179"/>
+      <c r="C53" s="179"/>
+      <c r="D53" s="179"/>
+      <c r="E53" s="179"/>
+      <c r="F53" s="179"/>
       <c r="G53" s="16">
         <f>SUM(H43:H52)</f>
         <v>0</v>
@@ -8225,18 +8223,18 @@
       <c r="N53" s="4"/>
     </row>
     <row r="54" spans="1:17" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="210" t="s">
+      <c r="A54" s="172" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="211"/>
-      <c r="C54" s="207" t="s">
+      <c r="B54" s="173"/>
+      <c r="C54" s="169" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="208"/>
-      <c r="E54" s="208"/>
-      <c r="F54" s="208"/>
-      <c r="G54" s="208"/>
-      <c r="H54" s="209"/>
+      <c r="D54" s="170"/>
+      <c r="E54" s="170"/>
+      <c r="F54" s="170"/>
+      <c r="G54" s="170"/>
+      <c r="H54" s="171"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -8307,14 +8305,14 @@
       <c r="Q56" s="93"/>
     </row>
     <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="189" t="s">
+      <c r="A57" s="178" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="190"/>
-      <c r="C57" s="190"/>
-      <c r="D57" s="190"/>
-      <c r="E57" s="190"/>
-      <c r="F57" s="190"/>
+      <c r="B57" s="179"/>
+      <c r="C57" s="179"/>
+      <c r="D57" s="179"/>
+      <c r="E57" s="179"/>
+      <c r="F57" s="179"/>
       <c r="G57" s="15">
         <f>SUM(H55:H56)</f>
         <v>0</v>
@@ -8331,16 +8329,16 @@
       <c r="N57" s="4"/>
     </row>
     <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="212" t="s">
+      <c r="A58" s="176" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="213"/>
-      <c r="C58" s="213"/>
-      <c r="D58" s="213"/>
-      <c r="E58" s="213"/>
-      <c r="F58" s="181"/>
-      <c r="G58" s="182"/>
-      <c r="H58" s="183"/>
+      <c r="B58" s="177"/>
+      <c r="C58" s="177"/>
+      <c r="D58" s="177"/>
+      <c r="E58" s="177"/>
+      <c r="F58" s="214"/>
+      <c r="G58" s="215"/>
+      <c r="H58" s="216"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -8349,14 +8347,14 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="171"/>
-      <c r="B59" s="172"/>
+      <c r="A59" s="204"/>
+      <c r="B59" s="205"/>
       <c r="C59" s="19"/>
-      <c r="D59" s="178" t="s">
+      <c r="D59" s="211" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="179"/>
-      <c r="F59" s="180"/>
+      <c r="E59" s="212"/>
+      <c r="F59" s="213"/>
       <c r="G59" s="20">
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
@@ -8370,13 +8368,13 @@
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="173"/>
-      <c r="B60" s="174"/>
+      <c r="A60" s="206"/>
+      <c r="B60" s="207"/>
       <c r="C60" s="22"/>
-      <c r="D60" s="175" t="s">
+      <c r="D60" s="208" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="176"/>
+      <c r="E60" s="209"/>
       <c r="F60" s="23"/>
       <c r="G60" s="24"/>
       <c r="H60" s="25"/>
@@ -8388,13 +8386,13 @@
       <c r="N60" s="4"/>
     </row>
     <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="173"/>
-      <c r="B61" s="174"/>
+      <c r="A61" s="206"/>
+      <c r="B61" s="207"/>
       <c r="C61" s="22"/>
-      <c r="D61" s="175" t="s">
+      <c r="D61" s="208" t="s">
         <v>56</v>
       </c>
-      <c r="E61" s="176"/>
+      <c r="E61" s="209"/>
       <c r="F61" s="23"/>
       <c r="G61" s="24"/>
       <c r="H61" s="25"/>
@@ -8406,13 +8404,13 @@
       <c r="N61" s="4"/>
     </row>
     <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="173"/>
-      <c r="B62" s="174"/>
+      <c r="A62" s="206"/>
+      <c r="B62" s="207"/>
       <c r="C62" s="26"/>
-      <c r="D62" s="177" t="s">
+      <c r="D62" s="210" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="176"/>
+      <c r="E62" s="209"/>
       <c r="F62" s="23"/>
       <c r="G62" s="24"/>
       <c r="H62" s="25"/>
@@ -8431,11 +8429,11 @@
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="169" t="s">
+      <c r="E63" s="202" t="s">
         <v>154</v>
       </c>
-      <c r="F63" s="169"/>
-      <c r="G63" s="170"/>
+      <c r="F63" s="202"/>
+      <c r="G63" s="203"/>
       <c r="H63" s="34"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -8445,10 +8443,10 @@
       <c r="N63" s="4"/>
     </row>
     <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="163" t="s">
+      <c r="A64" s="200" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="164"/>
+      <c r="B64" s="201"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
       <c r="E64" s="35"/>
@@ -8522,17 +8520,22 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="43">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="C42:H42"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A41:F41"/>
     <mergeCell ref="A2:B2"/>
@@ -8549,22 +8552,17 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="F43:F52 F55:F56 F13:F26 F29:F40">
     <cfRule type="cellIs" dxfId="42" priority="371" operator="equal">
@@ -9618,15 +9616,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
@@ -9647,57 +9636,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B7F6C1E041661428C0804F60FDF9579" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="269e77b516f09928499b1be999970057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17eb8759-252b-418d-a649-70aff91fc5df" xmlns:ns3="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720" xmlns:ns4="93977a9a-7c70-4c47-a38b-6f123b62dce6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41b65eea62d023978f15f5547645abd7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="17eb8759-252b-418d-a649-70aff91fc5df"/>
@@ -9918,15 +9866,57 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -9944,15 +9934,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5CD16F-1A82-4BAB-88E6-9D42833A2748}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9970,4 +9960,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Require Manual Testing to the AODA Report
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/WATR_Template.xlsx
+++ b/AxeAccessibilityDriver/WATR_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31067212-021C-4A5D-88F4-B9B9F6073F2D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAD5378-B98E-4942-A484-FECC775CA961}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="250">
   <si>
     <t>1.1.1</t>
   </si>
@@ -2396,6 +2396,9 @@
   </si>
   <si>
     <t>AA</t>
+  </si>
+  <si>
+    <t>Requires Manual Testing</t>
   </si>
 </sst>
 </file>
@@ -3669,121 +3672,22 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3826,6 +3730,105 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5184,7 +5187,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:IR30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -6725,10 +6728,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:XFC81"/>
+  <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -6738,31 +6741,25 @@
     <col min="3" max="3" width="10.7109375" style="28" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" style="29" customWidth="1"/>
     <col min="5" max="5" width="85.85546875" style="36" customWidth="1"/>
-    <col min="6" max="7" width="0" style="28" hidden="1"/>
-    <col min="8" max="8" width="0" style="27" hidden="1"/>
+    <col min="6" max="7" width="9.140625" style="28" hidden="1"/>
+    <col min="8" max="8" width="9.140625" style="27" hidden="1"/>
     <col min="9" max="16" width="0" style="5" hidden="1"/>
     <col min="17" max="17" width="0" style="6" hidden="1"/>
     <col min="18" max="19" width="0" style="5" hidden="1"/>
-    <col min="20" max="16378" width="85.85546875" style="5" hidden="1"/>
-    <col min="16379" max="16379" width="25.7109375" style="5" hidden="1"/>
-    <col min="16380" max="16380" width="28.42578125" style="5" hidden="1"/>
-    <col min="16381" max="16381" width="34" style="5" hidden="1"/>
-    <col min="16382" max="16382" width="29.28515625" style="5" hidden="1"/>
-    <col min="16383" max="16383" width="16.5703125" style="5" hidden="1"/>
-    <col min="16384" max="16384" width="85.85546875" style="5" hidden="1"/>
+    <col min="20" max="16384" width="9.140625" style="5" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="180" t="s">
+      <c r="A1" s="187" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="181"/>
+      <c r="B1" s="187"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="188"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
@@ -6776,13 +6773,13 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="168" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="182"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="184"/>
+      <c r="B2" s="168"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="192"/>
       <c r="F2" s="30"/>
       <c r="G2" s="1"/>
       <c r="H2" s="7"/>
@@ -6794,13 +6791,13 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="182" t="s">
+      <c r="A3" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="182"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="199"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="205"/>
+      <c r="E3" s="206"/>
       <c r="F3" s="30"/>
       <c r="G3" s="1"/>
       <c r="H3" s="7"/>
@@ -6812,12 +6809,12 @@
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="182" t="s">
+      <c r="A4" s="168" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="182"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
+      <c r="B4" s="168"/>
+      <c r="C4" s="214"/>
+      <c r="D4" s="214"/>
       <c r="E4" s="82"/>
       <c r="F4" s="30"/>
       <c r="G4" s="1"/>
@@ -6830,13 +6827,13 @@
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="164" t="s">
+      <c r="A5" s="167" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="164"/>
-      <c r="C5" s="165"/>
-      <c r="D5" s="165"/>
-      <c r="E5" s="166"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="215"/>
+      <c r="D5" s="215"/>
+      <c r="E5" s="216"/>
       <c r="F5" s="30"/>
       <c r="G5" s="1"/>
       <c r="H5" s="7"/>
@@ -6848,13 +6845,13 @@
       <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="164" t="s">
+      <c r="A6" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="164"/>
-      <c r="C6" s="167"/>
-      <c r="D6" s="167"/>
-      <c r="E6" s="168"/>
+      <c r="B6" s="167"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="166"/>
       <c r="F6" s="30"/>
       <c r="G6" s="1"/>
       <c r="H6" s="7"/>
@@ -6866,13 +6863,13 @@
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="164" t="s">
+      <c r="A7" s="167" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="164"/>
-      <c r="C7" s="167"/>
-      <c r="D7" s="167"/>
-      <c r="E7" s="168"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="166"/>
       <c r="F7" s="30"/>
       <c r="G7" s="1"/>
       <c r="H7" s="7"/>
@@ -6884,13 +6881,13 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="167" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="164"/>
-      <c r="C8" s="167"/>
-      <c r="D8" s="167"/>
-      <c r="E8" s="168"/>
+      <c r="B8" s="167"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="166"/>
       <c r="F8" s="30"/>
       <c r="G8" s="1"/>
       <c r="H8" s="7"/>
@@ -6902,16 +6899,16 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:19" s="28" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="186" t="s">
+      <c r="A9" s="195" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="187"/>
-      <c r="C9" s="187"/>
-      <c r="D9" s="187"/>
-      <c r="E9" s="187"/>
-      <c r="F9" s="187"/>
-      <c r="G9" s="187"/>
-      <c r="H9" s="187"/>
+      <c r="B9" s="196"/>
+      <c r="C9" s="196"/>
+      <c r="D9" s="196"/>
+      <c r="E9" s="196"/>
+      <c r="F9" s="196"/>
+      <c r="G9" s="196"/>
+      <c r="H9" s="196"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -6921,16 +6918,16 @@
       <c r="Q9" s="99"/>
     </row>
     <row r="10" spans="1:19" s="13" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="188" t="s">
+      <c r="A10" s="197" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="189"/>
-      <c r="C10" s="189"/>
-      <c r="D10" s="189"/>
-      <c r="E10" s="189"/>
-      <c r="F10" s="189"/>
-      <c r="G10" s="189"/>
-      <c r="H10" s="190"/>
+      <c r="B10" s="198"/>
+      <c r="C10" s="198"/>
+      <c r="D10" s="198"/>
+      <c r="E10" s="198"/>
+      <c r="F10" s="198"/>
+      <c r="G10" s="198"/>
+      <c r="H10" s="199"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -6940,10 +6937,10 @@
       <c r="Q10" s="14"/>
     </row>
     <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="195" t="s">
+      <c r="A11" s="202" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="196"/>
+      <c r="B11" s="203"/>
       <c r="C11" s="105" t="s">
         <v>40</v>
       </c>
@@ -6953,10 +6950,10 @@
       <c r="E11" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="191" t="s">
+      <c r="F11" s="201" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="191"/>
+      <c r="G11" s="201"/>
       <c r="H11" s="106" t="s">
         <v>53</v>
       </c>
@@ -6968,18 +6965,18 @@
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="174" t="s">
+      <c r="A12" s="193" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="185"/>
-      <c r="C12" s="192" t="s">
+      <c r="B12" s="194"/>
+      <c r="C12" s="184" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="193"/>
-      <c r="E12" s="193"/>
-      <c r="F12" s="193"/>
-      <c r="G12" s="193"/>
-      <c r="H12" s="194"/>
+      <c r="D12" s="185"/>
+      <c r="E12" s="185"/>
+      <c r="F12" s="185"/>
+      <c r="G12" s="185"/>
+      <c r="H12" s="186"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -7007,7 +7004,7 @@
       </c>
       <c r="G13" s="89"/>
       <c r="H13" s="90">
-        <f>IF(D13="Pass",0,IF(D13="criteria not applicable",0,IF(D13="Fail",1,"")))</f>
+        <f>IF(D13="Fail",1,0)</f>
         <v>0</v>
       </c>
       <c r="I13" s="91"/>
@@ -7038,7 +7035,7 @@
       </c>
       <c r="G14" s="89"/>
       <c r="H14" s="90">
-        <f t="shared" ref="H14:H26" si="0">IF(D14="Pass",0,IF(D14="criteria not applicable",0,IF(D14="Fail",1,"")))</f>
+        <f t="shared" ref="H14:H26" si="0">IF(D14="Fail",1,0)</f>
         <v>0</v>
       </c>
       <c r="I14" s="91"/>
@@ -7217,7 +7214,7 @@
         <v>247</v>
       </c>
       <c r="D20" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E20" s="162"/>
       <c r="F20" s="88">
@@ -7292,7 +7289,7 @@
       </c>
       <c r="G22" s="89"/>
       <c r="H22" s="90">
-        <f t="shared" si="0"/>
+        <f>IF(D22="Fail",1,0)</f>
         <v>0</v>
       </c>
       <c r="I22" s="91"/>
@@ -7334,7 +7331,9 @@
       <c r="L23" s="91"/>
       <c r="M23" s="91"/>
       <c r="N23" s="91"/>
-      <c r="Q23" s="93"/>
+      <c r="Q23" s="93" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="24" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="83" t="s">
@@ -7380,7 +7379,7 @@
         <v>248</v>
       </c>
       <c r="D25" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E25" s="162"/>
       <c r="F25" s="88">
@@ -7411,7 +7410,7 @@
         <v>248</v>
       </c>
       <c r="D26" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E26" s="162"/>
       <c r="F26" s="88">
@@ -7432,14 +7431,14 @@
       <c r="Q26" s="93"/>
     </row>
     <row r="27" spans="1:17" ht="17.45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="178" t="s">
+      <c r="A27" s="189" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="179"/>
-      <c r="C27" s="179"/>
-      <c r="D27" s="179"/>
-      <c r="E27" s="179"/>
-      <c r="F27" s="179"/>
+      <c r="B27" s="190"/>
+      <c r="C27" s="190"/>
+      <c r="D27" s="190"/>
+      <c r="E27" s="190"/>
+      <c r="F27" s="190"/>
       <c r="G27" s="15">
         <f>SUM(H13:H26)</f>
         <v>0</v>
@@ -7456,18 +7455,18 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="174" t="s">
+      <c r="A28" s="193" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="175"/>
-      <c r="C28" s="192" t="s">
+      <c r="B28" s="200"/>
+      <c r="C28" s="184" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="193"/>
-      <c r="E28" s="193"/>
-      <c r="F28" s="193"/>
-      <c r="G28" s="193"/>
-      <c r="H28" s="194"/>
+      <c r="D28" s="185"/>
+      <c r="E28" s="185"/>
+      <c r="F28" s="185"/>
+      <c r="G28" s="185"/>
+      <c r="H28" s="186"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -7486,7 +7485,7 @@
         <v>247</v>
       </c>
       <c r="D29" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E29" s="162"/>
       <c r="F29" s="88">
@@ -7495,7 +7494,7 @@
       </c>
       <c r="G29" s="89"/>
       <c r="H29" s="90">
-        <f>IF(D29="Pass",0,IF(D29="criteria not applicable",0,IF(D29="Fail",1,"")))</f>
+        <f t="shared" ref="H29:H40" si="3">IF(D29="Fail",1,0)</f>
         <v>0</v>
       </c>
       <c r="I29" s="91"/>
@@ -7517,7 +7516,7 @@
         <v>247</v>
       </c>
       <c r="D30" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E30" s="162"/>
       <c r="F30" s="88">
@@ -7526,7 +7525,7 @@
       </c>
       <c r="G30" s="89"/>
       <c r="H30" s="90">
-        <f t="shared" ref="H30:H40" si="3">IF(D30="Pass",0,IF(D30="criteria not applicable",0,IF(D30="Fail",1,"")))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I30" s="91"/>
@@ -7700,7 +7699,7 @@
         <v>247</v>
       </c>
       <c r="D36" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E36" s="162"/>
       <c r="F36" s="88">
@@ -7824,7 +7823,7 @@
         <v>248</v>
       </c>
       <c r="D40" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E40" s="162"/>
       <c r="F40" s="88">
@@ -7845,14 +7844,14 @@
       <c r="Q40" s="93"/>
     </row>
     <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="178" t="s">
+      <c r="A41" s="189" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="179"/>
-      <c r="C41" s="179"/>
-      <c r="D41" s="179"/>
-      <c r="E41" s="179"/>
-      <c r="F41" s="179"/>
+      <c r="B41" s="190"/>
+      <c r="C41" s="190"/>
+      <c r="D41" s="190"/>
+      <c r="E41" s="190"/>
+      <c r="F41" s="190"/>
       <c r="G41" s="15">
         <f>SUM(H29:H40)</f>
         <v>0</v>
@@ -7869,18 +7868,18 @@
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="174" t="s">
+      <c r="A42" s="193" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="175"/>
-      <c r="C42" s="192" t="s">
+      <c r="B42" s="200"/>
+      <c r="C42" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="193"/>
-      <c r="E42" s="193"/>
-      <c r="F42" s="193"/>
-      <c r="G42" s="193"/>
-      <c r="H42" s="194"/>
+      <c r="D42" s="185"/>
+      <c r="E42" s="185"/>
+      <c r="F42" s="185"/>
+      <c r="G42" s="185"/>
+      <c r="H42" s="186"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -7908,7 +7907,7 @@
       </c>
       <c r="G43" s="89"/>
       <c r="H43" s="90">
-        <f>IF(D43="Pass",0,IF(D43="criteria not applicable",0,IF(D43="Fail",1,"")))</f>
+        <f t="shared" ref="H43:H52" si="5">IF(D43="Fail",1,0)</f>
         <v>0</v>
       </c>
       <c r="I43" s="91"/>
@@ -7939,7 +7938,7 @@
       </c>
       <c r="G44" s="89"/>
       <c r="H44" s="90">
-        <f t="shared" ref="H44:H52" si="5">IF(D44="Pass",0,IF(D44="criteria not applicable",0,IF(D44="Fail",1,"")))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I44" s="91"/>
@@ -7961,7 +7960,7 @@
         <v>247</v>
       </c>
       <c r="D45" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E45" s="162"/>
       <c r="F45" s="88">
@@ -8085,7 +8084,7 @@
         <v>247</v>
       </c>
       <c r="D49" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E49" s="162"/>
       <c r="F49" s="88">
@@ -8147,7 +8146,7 @@
         <v>248</v>
       </c>
       <c r="D51" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E51" s="162"/>
       <c r="F51" s="88">
@@ -8199,14 +8198,14 @@
       <c r="Q52" s="93"/>
     </row>
     <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="178" t="s">
+      <c r="A53" s="189" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="179"/>
-      <c r="C53" s="179"/>
-      <c r="D53" s="179"/>
-      <c r="E53" s="179"/>
-      <c r="F53" s="179"/>
+      <c r="B53" s="190"/>
+      <c r="C53" s="190"/>
+      <c r="D53" s="190"/>
+      <c r="E53" s="190"/>
+      <c r="F53" s="190"/>
       <c r="G53" s="16">
         <f>SUM(H43:H52)</f>
         <v>0</v>
@@ -8223,18 +8222,18 @@
       <c r="N53" s="4"/>
     </row>
     <row r="54" spans="1:17" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="172" t="s">
+      <c r="A54" s="210" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="173"/>
-      <c r="C54" s="169" t="s">
+      <c r="B54" s="211"/>
+      <c r="C54" s="207" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="170"/>
-      <c r="E54" s="170"/>
-      <c r="F54" s="170"/>
-      <c r="G54" s="170"/>
-      <c r="H54" s="171"/>
+      <c r="D54" s="208"/>
+      <c r="E54" s="208"/>
+      <c r="F54" s="208"/>
+      <c r="G54" s="208"/>
+      <c r="H54" s="209"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -8262,7 +8261,7 @@
       </c>
       <c r="G55" s="89"/>
       <c r="H55" s="90">
-        <f>IF(D55="Pass",0,IF(D55="criteria not applicable",0,IF(D55="Fail",1,"")))</f>
+        <f t="shared" ref="H55:H56" si="6">IF(D55="Fail",1,0)</f>
         <v>0</v>
       </c>
       <c r="I55" s="91"/>
@@ -8293,7 +8292,7 @@
       </c>
       <c r="G56" s="89"/>
       <c r="H56" s="90">
-        <f>IF(D56="Pass",0,IF(D56="criteria not applicable",0,IF(D56="Fail",1,"")))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I56" s="91"/>
@@ -8305,14 +8304,14 @@
       <c r="Q56" s="93"/>
     </row>
     <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="178" t="s">
+      <c r="A57" s="189" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="179"/>
-      <c r="C57" s="179"/>
-      <c r="D57" s="179"/>
-      <c r="E57" s="179"/>
-      <c r="F57" s="179"/>
+      <c r="B57" s="190"/>
+      <c r="C57" s="190"/>
+      <c r="D57" s="190"/>
+      <c r="E57" s="190"/>
+      <c r="F57" s="190"/>
       <c r="G57" s="15">
         <f>SUM(H55:H56)</f>
         <v>0</v>
@@ -8329,16 +8328,16 @@
       <c r="N57" s="4"/>
     </row>
     <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="176" t="s">
+      <c r="A58" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="177"/>
-      <c r="C58" s="177"/>
-      <c r="D58" s="177"/>
-      <c r="E58" s="177"/>
-      <c r="F58" s="214"/>
-      <c r="G58" s="215"/>
-      <c r="H58" s="216"/>
+      <c r="B58" s="213"/>
+      <c r="C58" s="213"/>
+      <c r="D58" s="213"/>
+      <c r="E58" s="213"/>
+      <c r="F58" s="181"/>
+      <c r="G58" s="182"/>
+      <c r="H58" s="183"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -8347,14 +8346,14 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="204"/>
-      <c r="B59" s="205"/>
+      <c r="A59" s="171"/>
+      <c r="B59" s="172"/>
       <c r="C59" s="19"/>
-      <c r="D59" s="211" t="s">
+      <c r="D59" s="178" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="212"/>
-      <c r="F59" s="213"/>
+      <c r="E59" s="179"/>
+      <c r="F59" s="180"/>
       <c r="G59" s="20">
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
@@ -8368,13 +8367,13 @@
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="206"/>
-      <c r="B60" s="207"/>
+      <c r="A60" s="173"/>
+      <c r="B60" s="174"/>
       <c r="C60" s="22"/>
-      <c r="D60" s="208" t="s">
+      <c r="D60" s="175" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="209"/>
+      <c r="E60" s="176"/>
       <c r="F60" s="23"/>
       <c r="G60" s="24"/>
       <c r="H60" s="25"/>
@@ -8386,13 +8385,13 @@
       <c r="N60" s="4"/>
     </row>
     <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="206"/>
-      <c r="B61" s="207"/>
+      <c r="A61" s="173"/>
+      <c r="B61" s="174"/>
       <c r="C61" s="22"/>
-      <c r="D61" s="208" t="s">
+      <c r="D61" s="175" t="s">
         <v>56</v>
       </c>
-      <c r="E61" s="209"/>
+      <c r="E61" s="176"/>
       <c r="F61" s="23"/>
       <c r="G61" s="24"/>
       <c r="H61" s="25"/>
@@ -8404,13 +8403,13 @@
       <c r="N61" s="4"/>
     </row>
     <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="206"/>
-      <c r="B62" s="207"/>
+      <c r="A62" s="173"/>
+      <c r="B62" s="174"/>
       <c r="C62" s="26"/>
-      <c r="D62" s="210" t="s">
+      <c r="D62" s="177" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="209"/>
+      <c r="E62" s="176"/>
       <c r="F62" s="23"/>
       <c r="G62" s="24"/>
       <c r="H62" s="25"/>
@@ -8429,11 +8428,11 @@
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="202" t="s">
+      <c r="E63" s="169" t="s">
         <v>154</v>
       </c>
-      <c r="F63" s="202"/>
-      <c r="G63" s="203"/>
+      <c r="F63" s="169"/>
+      <c r="G63" s="170"/>
       <c r="H63" s="34"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -8443,10 +8442,10 @@
       <c r="N63" s="4"/>
     </row>
     <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="200" t="s">
+      <c r="A64" s="163" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="201"/>
+      <c r="B64" s="164"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
       <c r="E64" s="35"/>
@@ -8520,6 +8519,33 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="43">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="A8:B8"/>
@@ -8536,33 +8562,6 @@
     <mergeCell ref="D59:F59"/>
     <mergeCell ref="F58:H58"/>
     <mergeCell ref="C42:H42"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="F43:F52 F55:F56 F13:F26 F29:F40">
     <cfRule type="cellIs" dxfId="42" priority="371" operator="equal">
@@ -8724,8 +8723,8 @@
   </conditionalFormatting>
   <dataValidations xWindow="1400" yWindow="731" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="anticipated date of compliance. Format: M/DD/YYYY" sqref="G13:G26 G29:G40 G43:G52 G55:G56" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D43:D52 D29:D40 D13:D26 D55:D56" xr:uid="{00000000-0002-0000-0200-000001000000}">
-      <formula1>$Q$20:$Q$22</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D43:D52 D55:D56 D13:D26 D29:D40" xr:uid="{00000000-0002-0000-0200-000001000000}">
+      <formula1>$Q$20:$Q$23</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -9616,6 +9615,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
@@ -9636,16 +9644,57 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B7F6C1E041661428C0804F60FDF9579" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="269e77b516f09928499b1be999970057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17eb8759-252b-418d-a649-70aff91fc5df" xmlns:ns3="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720" xmlns:ns4="93977a9a-7c70-4c47-a38b-6f123b62dce6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41b65eea62d023978f15f5547645abd7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="17eb8759-252b-418d-a649-70aff91fc5df"/>
@@ -9866,57 +9915,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -9934,15 +9941,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5CD16F-1A82-4BAB-88E6-9D42833A2748}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9960,12 +9967,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changed summary sheet default value
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/WATR_Template.xlsx
+++ b/AxeAccessibilityDriver/WATR_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DuongCh\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAD5378-B98E-4942-A484-FECC775CA961}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469A9BEC-54DC-408D-B86D-CBC5F72656B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -3672,22 +3672,121 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="13" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3730,105 +3829,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4674,15 +4674,15 @@
       <selection activeCell="A47" sqref="A47:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.3" zeroHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="153.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="50" hidden="1" customWidth="1"/>
-    <col min="3" max="7" width="8.85546875" style="50" hidden="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="153.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="50" hidden="1" customWidth="1"/>
+    <col min="3" max="7" width="8.83203125" style="50" hidden="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="51" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="51" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="54" t="s">
         <v>157</v>
       </c>
@@ -4693,7 +4693,7 @@
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
     </row>
-    <row r="2" spans="1:7" s="51" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="51" customFormat="1" ht="28.2" x14ac:dyDescent="0.5">
       <c r="A2" s="65" t="s">
         <v>221</v>
       </c>
@@ -4704,7 +4704,7 @@
       <c r="F2" s="49"/>
       <c r="G2" s="49"/>
     </row>
-    <row r="3" spans="1:7" s="65" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="65" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="62" t="s">
         <v>213</v>
       </c>
@@ -4715,7 +4715,7 @@
       <c r="F3" s="64"/>
       <c r="G3" s="64"/>
     </row>
-    <row r="4" spans="1:7" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="62" t="s">
         <v>222</v>
       </c>
@@ -4726,7 +4726,7 @@
       <c r="F4" s="64"/>
       <c r="G4" s="64"/>
     </row>
-    <row r="5" spans="1:7" s="65" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="65" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A5" s="111" t="s">
         <v>219</v>
       </c>
@@ -4737,7 +4737,7 @@
       <c r="F5" s="64"/>
       <c r="G5" s="64"/>
     </row>
-    <row r="6" spans="1:7" s="65" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="65" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="66" t="s">
         <v>160</v>
       </c>
@@ -4748,7 +4748,7 @@
       <c r="F6" s="64"/>
       <c r="G6" s="64"/>
     </row>
-    <row r="7" spans="1:7" s="65" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="65" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="67" t="s">
         <v>145</v>
       </c>
@@ -4759,7 +4759,7 @@
       <c r="F7" s="64"/>
       <c r="G7" s="64"/>
     </row>
-    <row r="8" spans="1:7" s="65" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="65" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="67"/>
       <c r="B8" s="63"/>
       <c r="C8" s="64"/>
@@ -4768,7 +4768,7 @@
       <c r="F8" s="64"/>
       <c r="G8" s="64"/>
     </row>
-    <row r="9" spans="1:7" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="A9" s="68" t="s">
         <v>148</v>
       </c>
@@ -4779,7 +4779,7 @@
       <c r="F9" s="64"/>
       <c r="G9" s="64"/>
     </row>
-    <row r="10" spans="1:7" s="65" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="65" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="67" t="s">
         <v>149</v>
       </c>
@@ -4790,7 +4790,7 @@
       <c r="F10" s="64"/>
       <c r="G10" s="64"/>
     </row>
-    <row r="11" spans="1:7" s="65" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="65" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="69" t="s">
         <v>167</v>
       </c>
@@ -4801,7 +4801,7 @@
       <c r="F11" s="64"/>
       <c r="G11" s="64"/>
     </row>
-    <row r="12" spans="1:7" s="65" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="65" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="70" t="s">
         <v>166</v>
       </c>
@@ -4812,7 +4812,7 @@
       <c r="F12" s="64"/>
       <c r="G12" s="64"/>
     </row>
-    <row r="13" spans="1:7" s="65" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="65" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="67" t="s">
         <v>142</v>
       </c>
@@ -4823,7 +4823,7 @@
       <c r="F13" s="64"/>
       <c r="G13" s="64"/>
     </row>
-    <row r="14" spans="1:7" s="65" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="65" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="67" t="s">
         <v>143</v>
       </c>
@@ -4834,7 +4834,7 @@
       <c r="F14" s="64"/>
       <c r="G14" s="64"/>
     </row>
-    <row r="15" spans="1:7" s="65" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="65" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="76" t="s">
         <v>146</v>
       </c>
@@ -4845,19 +4845,19 @@
       <c r="F15" s="64"/>
       <c r="G15" s="64"/>
     </row>
-    <row r="16" spans="1:7" s="52" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="52" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A16" s="56" t="s">
         <v>158</v>
       </c>
       <c r="B16" s="57"/>
     </row>
-    <row r="17" spans="1:7" s="71" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="71" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="68" t="s">
         <v>163</v>
       </c>
       <c r="B17" s="63"/>
     </row>
-    <row r="18" spans="1:7" s="65" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" s="65" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" s="67" t="s">
         <v>223</v>
       </c>
@@ -4868,7 +4868,7 @@
       <c r="F18" s="64"/>
       <c r="G18" s="64"/>
     </row>
-    <row r="19" spans="1:7" s="65" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" s="65" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="67" t="s">
         <v>168</v>
       </c>
@@ -4879,7 +4879,7 @@
       <c r="F19" s="64"/>
       <c r="G19" s="64"/>
     </row>
-    <row r="20" spans="1:7" s="109" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="109" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="67" t="s">
         <v>215</v>
       </c>
@@ -4890,7 +4890,7 @@
       <c r="F20" s="108"/>
       <c r="G20" s="108"/>
     </row>
-    <row r="21" spans="1:7" s="65" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="65" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="67" t="s">
         <v>169</v>
       </c>
@@ -4901,7 +4901,7 @@
       <c r="F21" s="64"/>
       <c r="G21" s="64"/>
     </row>
-    <row r="22" spans="1:7" s="65" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" s="65" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="67"/>
       <c r="B22" s="63"/>
       <c r="C22" s="64"/>
@@ -4910,7 +4910,7 @@
       <c r="F22" s="64"/>
       <c r="G22" s="64"/>
     </row>
-    <row r="23" spans="1:7" s="65" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" s="65" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A23" s="68" t="s">
         <v>214</v>
       </c>
@@ -4921,7 +4921,7 @@
       <c r="F23" s="64"/>
       <c r="G23" s="64"/>
     </row>
-    <row r="24" spans="1:7" s="65" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="65" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A24" s="67" t="s">
         <v>170</v>
       </c>
@@ -4932,7 +4932,7 @@
       <c r="F24" s="64"/>
       <c r="G24" s="64"/>
     </row>
-    <row r="25" spans="1:7" s="65" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="65" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" s="67" t="s">
         <v>171</v>
       </c>
@@ -4943,7 +4943,7 @@
       <c r="F25" s="64"/>
       <c r="G25" s="64"/>
     </row>
-    <row r="26" spans="1:7" s="65" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="65" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A26" s="67" t="s">
         <v>172</v>
       </c>
@@ -4954,7 +4954,7 @@
       <c r="F26" s="64"/>
       <c r="G26" s="64"/>
     </row>
-    <row r="27" spans="1:7" s="65" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" s="65" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A27" s="76" t="s">
         <v>159</v>
       </c>
@@ -4965,19 +4965,19 @@
       <c r="F27" s="64"/>
       <c r="G27" s="64"/>
     </row>
-    <row r="28" spans="1:7" s="52" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="52" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A28" s="56" t="s">
         <v>165</v>
       </c>
       <c r="B28" s="57"/>
     </row>
-    <row r="29" spans="1:7" s="52" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" s="52" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A29" s="58" t="s">
         <v>144</v>
       </c>
       <c r="B29" s="59"/>
     </row>
-    <row r="30" spans="1:7" s="65" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="65" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" s="68" t="s">
         <v>147</v>
       </c>
@@ -4988,7 +4988,7 @@
       <c r="F30" s="64"/>
       <c r="G30" s="64"/>
     </row>
-    <row r="31" spans="1:7" s="65" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="65" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A31" s="72" t="s">
         <v>211</v>
       </c>
@@ -4999,7 +4999,7 @@
       <c r="F31" s="64"/>
       <c r="G31" s="64"/>
     </row>
-    <row r="32" spans="1:7" s="65" customFormat="1" ht="97.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="65" customFormat="1" ht="97.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="77" t="s">
         <v>217</v>
       </c>
@@ -5010,19 +5010,19 @@
       <c r="F32" s="64"/>
       <c r="G32" s="64"/>
     </row>
-    <row r="33" spans="1:7" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="104" t="s">
         <v>173</v>
       </c>
       <c r="B33" s="53"/>
     </row>
-    <row r="34" spans="1:7" s="52" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" s="52" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A34" s="58" t="s">
         <v>150</v>
       </c>
       <c r="B34" s="60"/>
     </row>
-    <row r="35" spans="1:7" s="65" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" s="65" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A35" s="68" t="s">
         <v>164</v>
       </c>
@@ -5033,7 +5033,7 @@
       <c r="F35" s="64"/>
       <c r="G35" s="64"/>
     </row>
-    <row r="36" spans="1:7" s="65" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="65" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A36" s="68" t="s">
         <v>212</v>
       </c>
@@ -5044,7 +5044,7 @@
       <c r="F36" s="64"/>
       <c r="G36" s="64"/>
     </row>
-    <row r="37" spans="1:7" s="65" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="65" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A37" s="68" t="s">
         <v>216</v>
       </c>
@@ -5055,7 +5055,7 @@
       <c r="F37" s="64"/>
       <c r="G37" s="64"/>
     </row>
-    <row r="38" spans="1:7" s="65" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" s="65" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A38" s="72" t="s">
         <v>174</v>
       </c>
@@ -5066,7 +5066,7 @@
       <c r="F38" s="64"/>
       <c r="G38" s="64"/>
     </row>
-    <row r="39" spans="1:7" s="65" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="65" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A39" s="77" t="s">
         <v>161</v>
       </c>
@@ -5077,7 +5077,7 @@
       <c r="F39" s="64"/>
       <c r="G39" s="64"/>
     </row>
-    <row r="40" spans="1:7" s="65" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" s="65" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="110" t="s">
         <v>218</v>
       </c>
@@ -5088,13 +5088,13 @@
       <c r="F40" s="64"/>
       <c r="G40" s="64"/>
     </row>
-    <row r="41" spans="1:7" s="52" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" s="52" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A41" s="58" t="s">
         <v>153</v>
       </c>
       <c r="B41" s="60"/>
     </row>
-    <row r="42" spans="1:7" s="65" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" s="65" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A42" s="68" t="s">
         <v>155</v>
       </c>
@@ -5105,7 +5105,7 @@
       <c r="F42" s="64"/>
       <c r="G42" s="64"/>
     </row>
-    <row r="43" spans="1:7" s="65" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="65" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A43" s="68" t="s">
         <v>156</v>
       </c>
@@ -5116,7 +5116,7 @@
       <c r="F43" s="64"/>
       <c r="G43" s="64"/>
     </row>
-    <row r="44" spans="1:7" s="65" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" s="65" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A44" s="66" t="s">
         <v>162</v>
       </c>
@@ -5127,7 +5127,7 @@
       <c r="F44" s="64"/>
       <c r="G44" s="64"/>
     </row>
-    <row r="45" spans="1:7" s="65" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" s="65" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A45" s="66" t="s">
         <v>220</v>
       </c>
@@ -5138,7 +5138,7 @@
       <c r="F45" s="64"/>
       <c r="G45" s="64"/>
     </row>
-    <row r="46" spans="1:7" s="65" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" s="65" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="73" t="s">
         <v>175</v>
       </c>
@@ -5149,17 +5149,17 @@
       <c r="F46" s="64"/>
       <c r="G46" s="64"/>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
       <c r="A47" s="75" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="49" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="50" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="51" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="52" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="53" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="49" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="50" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="51" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="52" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="53" hidden="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -5191,17 +5191,17 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="194.7109375" style="127" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="122" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" style="123" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="41.7109375" style="115" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="194.71875" style="127" customWidth="1"/>
+    <col min="2" max="2" width="23.71875" style="122" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" style="123" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="41.71875" style="115" hidden="1" customWidth="1"/>
     <col min="5" max="252" width="0" style="118" hidden="1" customWidth="1"/>
-    <col min="253" max="16384" width="9.140625" style="43" hidden="1"/>
+    <col min="253" max="16384" width="9.1640625" style="43" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:252" s="41" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:252" s="41" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="103" t="s">
         <v>95</v>
       </c>
@@ -5219,7 +5219,7 @@
       <c r="M1" s="40"/>
       <c r="N1" s="40"/>
     </row>
-    <row r="2" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="79" t="s">
         <v>61</v>
       </c>
@@ -5233,7 +5233,7 @@
       <c r="H2" s="117"/>
       <c r="I2" s="117"/>
     </row>
-    <row r="3" spans="1:252" s="45" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:252" s="45" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="78" t="s">
         <v>94</v>
       </c>
@@ -5491,7 +5491,7 @@
       <c r="IQ3" s="121"/>
       <c r="IR3" s="121"/>
     </row>
-    <row r="4" spans="1:252" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:252" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="81"/>
       <c r="B4" s="46"/>
       <c r="C4" s="46"/>
@@ -5502,7 +5502,7 @@
       <c r="H4" s="117"/>
       <c r="I4" s="117"/>
     </row>
-    <row r="5" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="79" t="s">
         <v>91</v>
       </c>
@@ -5514,7 +5514,7 @@
       <c r="H5" s="117"/>
       <c r="I5" s="117"/>
     </row>
-    <row r="6" spans="1:252" s="45" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:252" s="45" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="78" t="s">
         <v>96</v>
       </c>
@@ -5770,7 +5770,7 @@
       <c r="IQ6" s="121"/>
       <c r="IR6" s="121"/>
     </row>
-    <row r="7" spans="1:252" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:252" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="81"/>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
@@ -5781,7 +5781,7 @@
       <c r="H7" s="117"/>
       <c r="I7" s="117"/>
     </row>
-    <row r="8" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="79" t="s">
         <v>92</v>
       </c>
@@ -5793,7 +5793,7 @@
       <c r="H8" s="117"/>
       <c r="I8" s="117"/>
     </row>
-    <row r="9" spans="1:252" s="45" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:252" s="45" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="78" t="s">
         <v>93</v>
       </c>
@@ -6049,7 +6049,7 @@
       <c r="IQ9" s="121"/>
       <c r="IR9" s="121"/>
     </row>
-    <row r="10" spans="1:252" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:252" ht="51.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="81" t="s">
         <v>245</v>
       </c>
@@ -6062,7 +6062,7 @@
       <c r="H10" s="117"/>
       <c r="I10" s="117"/>
     </row>
-    <row r="11" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="79" t="s">
         <v>90</v>
       </c>
@@ -6074,7 +6074,7 @@
       <c r="H11" s="117"/>
       <c r="I11" s="117"/>
     </row>
-    <row r="12" spans="1:252" s="45" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:252" s="45" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="80" t="s">
         <v>177</v>
       </c>
@@ -6330,7 +6330,7 @@
       <c r="IQ12" s="121"/>
       <c r="IR12" s="121"/>
     </row>
-    <row r="13" spans="1:252" ht="366.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:252" ht="366.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="81" t="s">
         <v>244</v>
       </c>
@@ -6343,7 +6343,7 @@
       <c r="H13" s="117"/>
       <c r="I13" s="117"/>
     </row>
-    <row r="14" spans="1:252" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:252" ht="35.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="79" t="s">
         <v>97</v>
       </c>
@@ -6355,7 +6355,7 @@
       <c r="H14" s="117"/>
       <c r="I14" s="117"/>
     </row>
-    <row r="15" spans="1:252" s="45" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:252" s="45" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="80" t="s">
         <v>98</v>
       </c>
@@ -6611,7 +6611,7 @@
       <c r="IQ15" s="121"/>
       <c r="IR15" s="121"/>
     </row>
-    <row r="16" spans="1:252" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:252" ht="171" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="81"/>
       <c r="B16" s="46"/>
       <c r="C16" s="46"/>
@@ -6622,7 +6622,7 @@
       <c r="H16" s="117"/>
       <c r="I16" s="117"/>
     </row>
-    <row r="17" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="79" t="s">
         <v>236</v>
       </c>
@@ -6634,7 +6634,7 @@
       <c r="H17" s="117"/>
       <c r="I17" s="117"/>
     </row>
-    <row r="18" spans="1:9" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="50.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="80" t="s">
         <v>237</v>
       </c>
@@ -6647,7 +6647,7 @@
       <c r="H18" s="117"/>
       <c r="I18" s="117"/>
     </row>
-    <row r="19" spans="1:9" ht="348" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="348" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="81"/>
       <c r="B19" s="42"/>
       <c r="C19" s="42"/>
@@ -6657,7 +6657,7 @@
       <c r="H19" s="117"/>
       <c r="I19" s="117"/>
     </row>
-    <row r="20" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="79" t="s">
         <v>238</v>
       </c>
@@ -6670,44 +6670,44 @@
       <c r="H20" s="117"/>
       <c r="I20" s="117"/>
     </row>
-    <row r="21" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="81" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="28.15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="79" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="81"/>
     </row>
-    <row r="24" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="124"/>
     </row>
-    <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="79" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="81" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="170.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="170.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="124"/>
     </row>
-    <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="79" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="125"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="126" t="s">
         <v>176</v>
       </c>
@@ -6730,36 +6730,36 @@
   </sheetPr>
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.3" zeroHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="27" customWidth="1"/>
-    <col min="2" max="2" width="88.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="28" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="85.85546875" style="36" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="28" hidden="1"/>
-    <col min="8" max="8" width="9.140625" style="27" hidden="1"/>
-    <col min="9" max="16" width="0" style="5" hidden="1"/>
-    <col min="17" max="17" width="0" style="6" hidden="1"/>
-    <col min="18" max="19" width="0" style="5" hidden="1"/>
-    <col min="20" max="16384" width="9.140625" style="5" hidden="1"/>
+    <col min="1" max="1" width="6.71875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="88.44140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.71875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" style="29" customWidth="1"/>
+    <col min="5" max="5" width="85.83203125" style="36" customWidth="1"/>
+    <col min="6" max="7" width="9.1640625" style="28" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="27" hidden="1" customWidth="1"/>
+    <col min="9" max="16" width="0" style="5" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="0" style="6" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="0" style="5" hidden="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.1640625" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="187" t="s">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="180" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-      <c r="H1" s="188"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="181"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
       <c r="K1" s="1"/>
@@ -6772,14 +6772,14 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="168" t="s">
+    <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="182" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="168"/>
-      <c r="C2" s="191"/>
-      <c r="D2" s="191"/>
-      <c r="E2" s="192"/>
+      <c r="B2" s="182"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="184"/>
       <c r="F2" s="30"/>
       <c r="G2" s="1"/>
       <c r="H2" s="7"/>
@@ -6790,14 +6790,14 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="168" t="s">
+    <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="182" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="168"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="205"/>
-      <c r="E3" s="206"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="199"/>
       <c r="F3" s="30"/>
       <c r="G3" s="1"/>
       <c r="H3" s="7"/>
@@ -6808,13 +6808,13 @@
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="168" t="s">
+    <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="182" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="168"/>
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
+      <c r="B4" s="182"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
       <c r="E4" s="82"/>
       <c r="F4" s="30"/>
       <c r="G4" s="1"/>
@@ -6826,14 +6826,14 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="167" t="s">
+    <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="164" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="167"/>
-      <c r="C5" s="215"/>
-      <c r="D5" s="215"/>
-      <c r="E5" s="216"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="166"/>
       <c r="F5" s="30"/>
       <c r="G5" s="1"/>
       <c r="H5" s="7"/>
@@ -6844,14 +6844,14 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="167" t="s">
+    <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="164" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="167"/>
-      <c r="C6" s="165"/>
-      <c r="D6" s="165"/>
-      <c r="E6" s="166"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
+      <c r="E6" s="168"/>
       <c r="F6" s="30"/>
       <c r="G6" s="1"/>
       <c r="H6" s="7"/>
@@ -6862,14 +6862,14 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="167" t="s">
+    <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="164" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="167"/>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="166"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="167"/>
+      <c r="E7" s="168"/>
       <c r="F7" s="30"/>
       <c r="G7" s="1"/>
       <c r="H7" s="7"/>
@@ -6880,14 +6880,14 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="167" t="s">
+    <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="164" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="167"/>
-      <c r="C8" s="165"/>
-      <c r="D8" s="165"/>
-      <c r="E8" s="166"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="167"/>
+      <c r="D8" s="167"/>
+      <c r="E8" s="168"/>
       <c r="F8" s="30"/>
       <c r="G8" s="1"/>
       <c r="H8" s="7"/>
@@ -6898,17 +6898,17 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:19" s="28" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="195" t="s">
+    <row r="9" spans="1:19" s="28" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="186" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="196"/>
-      <c r="C9" s="196"/>
-      <c r="D9" s="196"/>
-      <c r="E9" s="196"/>
-      <c r="F9" s="196"/>
-      <c r="G9" s="196"/>
-      <c r="H9" s="196"/>
+      <c r="B9" s="187"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="187"/>
+      <c r="E9" s="187"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="187"/>
+      <c r="H9" s="187"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -6917,17 +6917,17 @@
       <c r="N9" s="9"/>
       <c r="Q9" s="99"/>
     </row>
-    <row r="10" spans="1:19" s="13" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="197" t="s">
+    <row r="10" spans="1:19" s="13" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="188" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="198"/>
-      <c r="C10" s="198"/>
-      <c r="D10" s="198"/>
-      <c r="E10" s="198"/>
-      <c r="F10" s="198"/>
-      <c r="G10" s="198"/>
-      <c r="H10" s="199"/>
+      <c r="B10" s="189"/>
+      <c r="C10" s="189"/>
+      <c r="D10" s="189"/>
+      <c r="E10" s="189"/>
+      <c r="F10" s="189"/>
+      <c r="G10" s="189"/>
+      <c r="H10" s="190"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -6936,11 +6936,11 @@
       <c r="N10" s="12"/>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="202" t="s">
+    <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="195" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="203"/>
+      <c r="B11" s="196"/>
       <c r="C11" s="105" t="s">
         <v>40</v>
       </c>
@@ -6950,10 +6950,10 @@
       <c r="E11" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="201" t="s">
+      <c r="F11" s="191" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="201"/>
+      <c r="G11" s="191"/>
       <c r="H11" s="106" t="s">
         <v>53</v>
       </c>
@@ -6964,19 +6964,19 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="193" t="s">
+    <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="174" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="194"/>
-      <c r="C12" s="184" t="s">
+      <c r="B12" s="185"/>
+      <c r="C12" s="192" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="185"/>
-      <c r="E12" s="185"/>
-      <c r="F12" s="185"/>
-      <c r="G12" s="185"/>
-      <c r="H12" s="186"/>
+      <c r="D12" s="193"/>
+      <c r="E12" s="193"/>
+      <c r="F12" s="193"/>
+      <c r="G12" s="193"/>
+      <c r="H12" s="194"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -6984,7 +6984,7 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:19" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A13" s="83" t="s">
         <v>0</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>247</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E13" s="162"/>
       <c r="F13" s="88">
@@ -7015,7 +7015,7 @@
       <c r="N13" s="91"/>
       <c r="Q13" s="93"/>
     </row>
-    <row r="14" spans="1:19" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A14" s="83" t="s">
         <v>1</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>247</v>
       </c>
       <c r="D14" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E14" s="162"/>
       <c r="F14" s="88">
@@ -7046,7 +7046,7 @@
       <c r="N14" s="91"/>
       <c r="Q14" s="93"/>
     </row>
-    <row r="15" spans="1:19" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A15" s="83" t="s">
         <v>2</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>247</v>
       </c>
       <c r="D15" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E15" s="162"/>
       <c r="F15" s="88">
@@ -7077,7 +7077,7 @@
       <c r="N15" s="91"/>
       <c r="Q15" s="93"/>
     </row>
-    <row r="16" spans="1:19" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A16" s="83" t="s">
         <v>3</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v>247</v>
       </c>
       <c r="D16" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E16" s="162"/>
       <c r="F16" s="88">
@@ -7108,7 +7108,7 @@
       <c r="N16" s="91"/>
       <c r="Q16" s="93"/>
     </row>
-    <row r="17" spans="1:17" s="92" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" s="92" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="A17" s="83" t="s">
         <v>4</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>248</v>
       </c>
       <c r="D17" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E17" s="162"/>
       <c r="F17" s="88">
@@ -7139,7 +7139,7 @@
       <c r="N17" s="91"/>
       <c r="Q17" s="93"/>
     </row>
-    <row r="18" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A18" s="83" t="s">
         <v>5</v>
       </c>
@@ -7150,7 +7150,7 @@
         <v>248</v>
       </c>
       <c r="D18" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E18" s="162"/>
       <c r="F18" s="88">
@@ -7170,7 +7170,7 @@
       <c r="N18" s="91"/>
       <c r="Q18" s="93"/>
     </row>
-    <row r="19" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A19" s="83" t="s">
         <v>6</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>247</v>
       </c>
       <c r="D19" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E19" s="162"/>
       <c r="F19" s="88">
@@ -7203,7 +7203,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="92" customFormat="1" ht="45.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A20" s="83" t="s">
         <v>7</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="92" customFormat="1" ht="45.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A21" s="83" t="s">
         <v>8</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>247</v>
       </c>
       <c r="D21" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E21" s="162"/>
       <c r="F21" s="88">
@@ -7269,7 +7269,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A22" s="83" t="s">
         <v>9</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>247</v>
       </c>
       <c r="D22" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E22" s="162"/>
       <c r="F22" s="88">
@@ -7302,7 +7302,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="92" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" s="92" customFormat="1" ht="60" x14ac:dyDescent="0.5">
       <c r="A23" s="83" t="s">
         <v>10</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>247</v>
       </c>
       <c r="D23" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E23" s="162"/>
       <c r="F23" s="88">
@@ -7335,7 +7335,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A24" s="83" t="s">
         <v>11</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>248</v>
       </c>
       <c r="D24" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E24" s="162"/>
       <c r="F24" s="88">
@@ -7368,7 +7368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A25" s="83" t="s">
         <v>12</v>
       </c>
@@ -7399,7 +7399,7 @@
       <c r="N25" s="91"/>
       <c r="Q25" s="93"/>
     </row>
-    <row r="26" spans="1:17" s="92" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" s="92" customFormat="1" ht="45.3" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="83" t="s">
         <v>13</v>
       </c>
@@ -7430,15 +7430,15 @@
       <c r="N26" s="91"/>
       <c r="Q26" s="93"/>
     </row>
-    <row r="27" spans="1:17" ht="17.45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="189" t="s">
+    <row r="27" spans="1:17" ht="17.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="178" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="190"/>
-      <c r="C27" s="190"/>
-      <c r="D27" s="190"/>
-      <c r="E27" s="190"/>
-      <c r="F27" s="190"/>
+      <c r="B27" s="179"/>
+      <c r="C27" s="179"/>
+      <c r="D27" s="179"/>
+      <c r="E27" s="179"/>
+      <c r="F27" s="179"/>
       <c r="G27" s="15">
         <f>SUM(H13:H26)</f>
         <v>0</v>
@@ -7454,19 +7454,19 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
     </row>
-    <row r="28" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="193" t="s">
+    <row r="28" spans="1:17" ht="53.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="174" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="200"/>
-      <c r="C28" s="184" t="s">
+      <c r="B28" s="175"/>
+      <c r="C28" s="192" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="185"/>
-      <c r="E28" s="185"/>
-      <c r="F28" s="185"/>
-      <c r="G28" s="185"/>
-      <c r="H28" s="186"/>
+      <c r="D28" s="193"/>
+      <c r="E28" s="193"/>
+      <c r="F28" s="193"/>
+      <c r="G28" s="193"/>
+      <c r="H28" s="194"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -7474,7 +7474,7 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" spans="1:17" s="92" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" s="92" customFormat="1" ht="60" x14ac:dyDescent="0.5">
       <c r="A29" s="83" t="s">
         <v>14</v>
       </c>
@@ -7505,7 +7505,7 @@
       <c r="N29" s="91"/>
       <c r="Q29" s="93"/>
     </row>
-    <row r="30" spans="1:17" s="92" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" s="92" customFormat="1" ht="75" x14ac:dyDescent="0.5">
       <c r="A30" s="83" t="s">
         <v>15</v>
       </c>
@@ -7536,7 +7536,7 @@
       <c r="N30" s="91"/>
       <c r="Q30" s="93"/>
     </row>
-    <row r="31" spans="1:17" s="92" customFormat="1" ht="210" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" s="92" customFormat="1" ht="210" x14ac:dyDescent="0.5">
       <c r="A31" s="83" t="s">
         <v>16</v>
       </c>
@@ -7547,7 +7547,7 @@
         <v>247</v>
       </c>
       <c r="D31" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E31" s="162"/>
       <c r="F31" s="88">
@@ -7567,7 +7567,7 @@
       <c r="N31" s="91"/>
       <c r="Q31" s="93"/>
     </row>
-    <row r="32" spans="1:17" s="92" customFormat="1" ht="150" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" s="92" customFormat="1" ht="150" x14ac:dyDescent="0.5">
       <c r="A32" s="83" t="s">
         <v>17</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>247</v>
       </c>
       <c r="D32" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E32" s="162"/>
       <c r="F32" s="88"/>
@@ -7595,7 +7595,7 @@
       <c r="N32" s="91"/>
       <c r="Q32" s="93"/>
     </row>
-    <row r="33" spans="1:17" s="92" customFormat="1" ht="45.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A33" s="83" t="s">
         <v>18</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>247</v>
       </c>
       <c r="D33" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E33" s="162"/>
       <c r="F33" s="88">
@@ -7626,7 +7626,7 @@
       <c r="N33" s="91"/>
       <c r="Q33" s="93"/>
     </row>
-    <row r="34" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A34" s="83" t="s">
         <v>19</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>247</v>
       </c>
       <c r="D34" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E34" s="162"/>
       <c r="F34" s="88">
@@ -7657,7 +7657,7 @@
       <c r="N34" s="91"/>
       <c r="Q34" s="93"/>
     </row>
-    <row r="35" spans="1:17" s="92" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" s="92" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="A35" s="83" t="s">
         <v>20</v>
       </c>
@@ -7668,7 +7668,7 @@
         <v>247</v>
       </c>
       <c r="D35" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E35" s="162"/>
       <c r="F35" s="88">
@@ -7688,7 +7688,7 @@
       <c r="N35" s="91"/>
       <c r="Q35" s="93"/>
     </row>
-    <row r="36" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A36" s="83" t="s">
         <v>21</v>
       </c>
@@ -7719,7 +7719,7 @@
       <c r="N36" s="91"/>
       <c r="Q36" s="93"/>
     </row>
-    <row r="37" spans="1:17" s="92" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A37" s="83" t="s">
         <v>22</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>247</v>
       </c>
       <c r="D37" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E37" s="162"/>
       <c r="F37" s="88">
@@ -7750,7 +7750,7 @@
       <c r="N37" s="91"/>
       <c r="Q37" s="93"/>
     </row>
-    <row r="38" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A38" s="83" t="s">
         <v>23</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>248</v>
       </c>
       <c r="D38" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E38" s="162"/>
       <c r="F38" s="88">
@@ -7781,7 +7781,7 @@
       <c r="N38" s="91"/>
       <c r="Q38" s="93"/>
     </row>
-    <row r="39" spans="1:17" s="92" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" s="92" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="A39" s="83" t="s">
         <v>24</v>
       </c>
@@ -7792,7 +7792,7 @@
         <v>248</v>
       </c>
       <c r="D39" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E39" s="162"/>
       <c r="F39" s="88">
@@ -7812,7 +7812,7 @@
       <c r="N39" s="91"/>
       <c r="Q39" s="93"/>
     </row>
-    <row r="40" spans="1:17" s="92" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="92" customFormat="1" ht="30.3" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="83" t="s">
         <v>25</v>
       </c>
@@ -7843,15 +7843,15 @@
       <c r="N40" s="91"/>
       <c r="Q40" s="93"/>
     </row>
-    <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="189" t="s">
+    <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="178" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="190"/>
-      <c r="C41" s="190"/>
-      <c r="D41" s="190"/>
-      <c r="E41" s="190"/>
-      <c r="F41" s="190"/>
+      <c r="B41" s="179"/>
+      <c r="C41" s="179"/>
+      <c r="D41" s="179"/>
+      <c r="E41" s="179"/>
+      <c r="F41" s="179"/>
       <c r="G41" s="15">
         <f>SUM(H29:H40)</f>
         <v>0</v>
@@ -7867,19 +7867,19 @@
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
     </row>
-    <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="193" t="s">
+    <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="174" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="200"/>
-      <c r="C42" s="184" t="s">
+      <c r="B42" s="175"/>
+      <c r="C42" s="192" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="185"/>
-      <c r="E42" s="185"/>
-      <c r="F42" s="185"/>
-      <c r="G42" s="185"/>
-      <c r="H42" s="186"/>
+      <c r="D42" s="193"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="193"/>
+      <c r="G42" s="193"/>
+      <c r="H42" s="194"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -7887,7 +7887,7 @@
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
     </row>
-    <row r="43" spans="1:17" s="92" customFormat="1" ht="30.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A43" s="83" t="s">
         <v>26</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>247</v>
       </c>
       <c r="D43" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E43" s="162"/>
       <c r="F43" s="88">
@@ -7918,7 +7918,7 @@
       <c r="N43" s="91"/>
       <c r="Q43" s="93"/>
     </row>
-    <row r="44" spans="1:17" s="92" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" s="92" customFormat="1" ht="60" x14ac:dyDescent="0.5">
       <c r="A44" s="83" t="s">
         <v>27</v>
       </c>
@@ -7929,7 +7929,7 @@
         <v>248</v>
       </c>
       <c r="D44" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E44" s="162"/>
       <c r="F44" s="88">
@@ -7949,7 +7949,7 @@
       <c r="N44" s="91"/>
       <c r="Q44" s="93"/>
     </row>
-    <row r="45" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A45" s="83" t="s">
         <v>28</v>
       </c>
@@ -7980,7 +7980,7 @@
       <c r="N45" s="91"/>
       <c r="Q45" s="93"/>
     </row>
-    <row r="46" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A46" s="83" t="s">
         <v>29</v>
       </c>
@@ -7991,7 +7991,7 @@
         <v>247</v>
       </c>
       <c r="D46" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E46" s="162"/>
       <c r="F46" s="88">
@@ -8011,7 +8011,7 @@
       <c r="N46" s="91"/>
       <c r="Q46" s="93"/>
     </row>
-    <row r="47" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A47" s="83" t="s">
         <v>30</v>
       </c>
@@ -8022,7 +8022,7 @@
         <v>248</v>
       </c>
       <c r="D47" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E47" s="162"/>
       <c r="F47" s="88">
@@ -8042,7 +8042,7 @@
       <c r="N47" s="91"/>
       <c r="Q47" s="93"/>
     </row>
-    <row r="48" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A48" s="83" t="s">
         <v>31</v>
       </c>
@@ -8053,7 +8053,7 @@
         <v>248</v>
       </c>
       <c r="D48" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E48" s="162"/>
       <c r="F48" s="88">
@@ -8073,7 +8073,7 @@
       <c r="N48" s="91"/>
       <c r="Q48" s="93"/>
     </row>
-    <row r="49" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A49" s="83" t="s">
         <v>32</v>
       </c>
@@ -8104,7 +8104,7 @@
       <c r="N49" s="91"/>
       <c r="Q49" s="93"/>
     </row>
-    <row r="50" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.5">
       <c r="A50" s="83" t="s">
         <v>33</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>247</v>
       </c>
       <c r="D50" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E50" s="162"/>
       <c r="F50" s="88">
@@ -8135,7 +8135,7 @@
       <c r="N50" s="91"/>
       <c r="Q50" s="93"/>
     </row>
-    <row r="51" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" s="92" customFormat="1" ht="45" x14ac:dyDescent="0.5">
       <c r="A51" s="83" t="s">
         <v>34</v>
       </c>
@@ -8166,7 +8166,7 @@
       <c r="N51" s="91"/>
       <c r="Q51" s="93"/>
     </row>
-    <row r="52" spans="1:17" s="92" customFormat="1" ht="136.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" s="92" customFormat="1" ht="135" x14ac:dyDescent="0.5">
       <c r="A52" s="83" t="s">
         <v>35</v>
       </c>
@@ -8177,7 +8177,7 @@
         <v>248</v>
       </c>
       <c r="D52" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E52" s="162"/>
       <c r="F52" s="88">
@@ -8197,15 +8197,15 @@
       <c r="N52" s="91"/>
       <c r="Q52" s="93"/>
     </row>
-    <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="189" t="s">
+    <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="178" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="190"/>
-      <c r="C53" s="190"/>
-      <c r="D53" s="190"/>
-      <c r="E53" s="190"/>
-      <c r="F53" s="190"/>
+      <c r="B53" s="179"/>
+      <c r="C53" s="179"/>
+      <c r="D53" s="179"/>
+      <c r="E53" s="179"/>
+      <c r="F53" s="179"/>
       <c r="G53" s="16">
         <f>SUM(H43:H52)</f>
         <v>0</v>
@@ -8221,19 +8221,19 @@
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
     </row>
-    <row r="54" spans="1:17" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="210" t="s">
+    <row r="54" spans="1:17" ht="47.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="172" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="211"/>
-      <c r="C54" s="207" t="s">
+      <c r="B54" s="173"/>
+      <c r="C54" s="169" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="208"/>
-      <c r="E54" s="208"/>
-      <c r="F54" s="208"/>
-      <c r="G54" s="208"/>
-      <c r="H54" s="209"/>
+      <c r="D54" s="170"/>
+      <c r="E54" s="170"/>
+      <c r="F54" s="170"/>
+      <c r="G54" s="170"/>
+      <c r="H54" s="171"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -8241,7 +8241,7 @@
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
     </row>
-    <row r="55" spans="1:17" s="92" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" s="92" customFormat="1" ht="60" x14ac:dyDescent="0.5">
       <c r="A55" s="83" t="s">
         <v>36</v>
       </c>
@@ -8252,7 +8252,7 @@
         <v>247</v>
       </c>
       <c r="D55" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E55" s="162"/>
       <c r="F55" s="88">
@@ -8272,7 +8272,7 @@
       <c r="N55" s="91"/>
       <c r="Q55" s="93"/>
     </row>
-    <row r="56" spans="1:17" s="92" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" s="92" customFormat="1" ht="75.3" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="83" t="s">
         <v>37</v>
       </c>
@@ -8283,7 +8283,7 @@
         <v>247</v>
       </c>
       <c r="D56" s="86" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="E56" s="162"/>
       <c r="F56" s="88">
@@ -8303,15 +8303,15 @@
       <c r="N56" s="91"/>
       <c r="Q56" s="93"/>
     </row>
-    <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="189" t="s">
+    <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="178" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="190"/>
-      <c r="C57" s="190"/>
-      <c r="D57" s="190"/>
-      <c r="E57" s="190"/>
-      <c r="F57" s="190"/>
+      <c r="B57" s="179"/>
+      <c r="C57" s="179"/>
+      <c r="D57" s="179"/>
+      <c r="E57" s="179"/>
+      <c r="F57" s="179"/>
       <c r="G57" s="15">
         <f>SUM(H55:H56)</f>
         <v>0</v>
@@ -8327,17 +8327,17 @@
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
     </row>
-    <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="212" t="s">
+    <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="176" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="213"/>
-      <c r="C58" s="213"/>
-      <c r="D58" s="213"/>
-      <c r="E58" s="213"/>
-      <c r="F58" s="181"/>
-      <c r="G58" s="182"/>
-      <c r="H58" s="183"/>
+      <c r="B58" s="177"/>
+      <c r="C58" s="177"/>
+      <c r="D58" s="177"/>
+      <c r="E58" s="177"/>
+      <c r="F58" s="214"/>
+      <c r="G58" s="215"/>
+      <c r="H58" s="216"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -8345,15 +8345,15 @@
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
     </row>
-    <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="171"/>
-      <c r="B59" s="172"/>
+    <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A59" s="204"/>
+      <c r="B59" s="205"/>
       <c r="C59" s="19"/>
-      <c r="D59" s="178" t="s">
+      <c r="D59" s="211" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="179"/>
-      <c r="F59" s="180"/>
+      <c r="E59" s="212"/>
+      <c r="F59" s="213"/>
       <c r="G59" s="20">
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
@@ -8366,14 +8366,14 @@
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
     </row>
-    <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="173"/>
-      <c r="B60" s="174"/>
+    <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="206"/>
+      <c r="B60" s="207"/>
       <c r="C60" s="22"/>
-      <c r="D60" s="175" t="s">
+      <c r="D60" s="208" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="176"/>
+      <c r="E60" s="209"/>
       <c r="F60" s="23"/>
       <c r="G60" s="24"/>
       <c r="H60" s="25"/>
@@ -8384,14 +8384,14 @@
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
     </row>
-    <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="173"/>
-      <c r="B61" s="174"/>
+    <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="206"/>
+      <c r="B61" s="207"/>
       <c r="C61" s="22"/>
-      <c r="D61" s="175" t="s">
+      <c r="D61" s="208" t="s">
         <v>56</v>
       </c>
-      <c r="E61" s="176"/>
+      <c r="E61" s="209"/>
       <c r="F61" s="23"/>
       <c r="G61" s="24"/>
       <c r="H61" s="25"/>
@@ -8402,14 +8402,14 @@
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
     </row>
-    <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="173"/>
-      <c r="B62" s="174"/>
+    <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="206"/>
+      <c r="B62" s="207"/>
       <c r="C62" s="26"/>
-      <c r="D62" s="177" t="s">
+      <c r="D62" s="210" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="176"/>
+      <c r="E62" s="209"/>
       <c r="F62" s="23"/>
       <c r="G62" s="24"/>
       <c r="H62" s="25"/>
@@ -8420,7 +8420,7 @@
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
     </row>
-    <row r="63" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="32"/>
       <c r="B63" s="61"/>
       <c r="C63" s="33"/>
@@ -8428,11 +8428,11 @@
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="169" t="s">
+      <c r="E63" s="202" t="s">
         <v>154</v>
       </c>
-      <c r="F63" s="169"/>
-      <c r="G63" s="170"/>
+      <c r="F63" s="202"/>
+      <c r="G63" s="203"/>
       <c r="H63" s="34"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -8441,11 +8441,11 @@
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
     </row>
-    <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="163" t="s">
+    <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A64" s="200" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="164"/>
+      <c r="B64" s="201"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
       <c r="E64" s="35"/>
@@ -8459,7 +8459,7 @@
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
     </row>
-    <row r="65" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="15" x14ac:dyDescent="0.5">
       <c r="A65" s="8"/>
       <c r="B65" s="102" t="s">
         <v>59</v>
@@ -8477,7 +8477,7 @@
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
     </row>
-    <row r="66" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="15" x14ac:dyDescent="0.5">
       <c r="A66" s="8"/>
       <c r="B66" s="102" t="s">
         <v>60</v>
@@ -8495,41 +8495,46 @@
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A67" s="100" t="s">
         <v>176</v>
       </c>
       <c r="B67" s="101"/>
       <c r="C67" s="98"/>
     </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="81" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="81" hidden="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="43">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="C42:H42"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A41:F41"/>
     <mergeCell ref="A2:B2"/>
@@ -8546,22 +8551,17 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="F43:F52 F55:F56 F13:F26 F29:F40">
     <cfRule type="cellIs" dxfId="42" priority="371" operator="equal">
@@ -8723,7 +8723,7 @@
   </conditionalFormatting>
   <dataValidations xWindow="1400" yWindow="731" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="anticipated date of compliance. Format: M/DD/YYYY" sqref="G13:G26 G29:G40 G43:G52 G55:G56" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D43:D52 D55:D56 D13:D26 D29:D40" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29:D40 D43:D52 D13:D26 D55:D56" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>$Q$20:$Q$23</formula1>
     </dataValidation>
   </dataValidations>
@@ -8759,246 +8759,246 @@
       <selection activeCell="A13" sqref="A13:A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="67.5703125" style="36" customWidth="1"/>
+    <col min="1" max="1" width="67.5546875" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1"/>
     </row>
-    <row r="2" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A2"/>
     </row>
-    <row r="3" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A3"/>
     </row>
-    <row r="4" spans="1:1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A4" s="82"/>
     </row>
-    <row r="5" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A5"/>
     </row>
-    <row r="6" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A6"/>
     </row>
-    <row r="7" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A8"/>
     </row>
-    <row r="9" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A10"/>
     </row>
-    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A11" s="105" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A12"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A13" s="113" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A14" s="87"/>
     </row>
-    <row r="15" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A15" s="87"/>
     </row>
-    <row r="16" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A16" s="87"/>
     </row>
-    <row r="17" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A17" s="87"/>
     </row>
-    <row r="18" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A18" s="87"/>
     </row>
-    <row r="19" spans="1:1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" ht="61.5" x14ac:dyDescent="0.4">
       <c r="A19" s="114" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" s="113"/>
     </row>
-    <row r="21" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" s="87"/>
     </row>
-    <row r="22" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A22" s="87"/>
     </row>
-    <row r="23" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A23" s="87"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A24" s="113" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A25" s="87" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A26" s="87"/>
     </row>
-    <row r="27" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A27"/>
     </row>
-    <row r="28" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28"/>
     </row>
-    <row r="29" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A29" s="87"/>
     </row>
-    <row r="30" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A30" s="87"/>
     </row>
-    <row r="31" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A31" s="87"/>
     </row>
-    <row r="32" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A32" s="87"/>
     </row>
-    <row r="33" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A33" s="87"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A34" s="113" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A35" s="87"/>
     </row>
-    <row r="36" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A36" s="87"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A37" s="113" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A38" s="87"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A39" s="113" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A40" s="87"/>
     </row>
-    <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A41"/>
     </row>
-    <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A42"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A43" s="113" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A44" s="87"/>
     </row>
-    <row r="45" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A45" s="87"/>
     </row>
-    <row r="46" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A46" s="87"/>
     </row>
-    <row r="47" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A47" s="87"/>
     </row>
-    <row r="48" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A48" s="87"/>
     </row>
-    <row r="49" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A49" s="87"/>
     </row>
-    <row r="50" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A50" s="87"/>
     </row>
-    <row r="51" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A51" s="87"/>
     </row>
-    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A52" s="113"/>
     </row>
-    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" ht="49.2" x14ac:dyDescent="0.4">
       <c r="A55" s="114" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="30" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A56" s="87" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A57"/>
     </row>
-    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A58"/>
     </row>
-    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A59"/>
     </row>
-    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A60"/>
     </row>
-    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A61"/>
     </row>
-    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A62"/>
     </row>
-    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A63"/>
     </row>
-    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A64" s="35"/>
     </row>
-    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A65" s="35"/>
     </row>
-    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A66" s="35"/>
     </row>
-    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="81" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="71" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="72" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="73" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="74" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="75" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="76" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="77" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="78" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="79" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="80" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
+    <row r="81" hidden="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <autoFilter ref="A1:A81" xr:uid="{8E9A06B2-A732-4118-A8AE-005B26054B05}">
     <filterColumn colId="0">
@@ -9056,21 +9056,21 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="134" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="134" customWidth="1"/>
-    <col min="3" max="3" width="76.28515625" style="134" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="134" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" style="134" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" style="160" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" style="134" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" style="134" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="134" hidden="1" customWidth="1"/>
-    <col min="10" max="16384" width="2.42578125" style="134" hidden="1"/>
+    <col min="1" max="1" width="10.44140625" style="134" customWidth="1"/>
+    <col min="2" max="2" width="24.27734375" style="134" customWidth="1"/>
+    <col min="3" max="3" width="76.27734375" style="134" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.27734375" style="134" customWidth="1"/>
+    <col min="5" max="5" width="56.71875" style="134" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" style="160" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" style="134" customWidth="1"/>
+    <col min="8" max="8" width="22.71875" style="134" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="134" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="2.44140625" style="134" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="130" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="130" customFormat="1" ht="17.7" x14ac:dyDescent="0.4">
       <c r="A1" s="218" t="s">
         <v>82</v>
       </c>
@@ -9091,7 +9091,7 @@
       <c r="P1" s="129"/>
       <c r="Q1" s="129"/>
     </row>
-    <row r="2" spans="1:20" s="135" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="135" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" s="217" t="s">
         <v>200</v>
       </c>
@@ -9113,7 +9113,7 @@
       </c>
       <c r="T2" s="132"/>
     </row>
-    <row r="3" spans="1:20" s="137" customFormat="1" ht="45.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="137" customFormat="1" ht="45" x14ac:dyDescent="0.4">
       <c r="A3" s="136" t="s">
         <v>75</v>
       </c>
@@ -9145,7 +9145,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="137" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" s="137" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="138"/>
       <c r="C4" s="161"/>
       <c r="D4" s="140"/>
@@ -9163,7 +9163,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B5" s="138"/>
       <c r="C5" s="147"/>
       <c r="D5" s="148"/>
@@ -9181,7 +9181,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B6" s="138"/>
       <c r="C6" s="147"/>
       <c r="D6" s="148"/>
@@ -9199,7 +9199,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B7" s="138"/>
       <c r="C7" s="147"/>
       <c r="D7" s="148"/>
@@ -9211,7 +9211,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B8" s="138"/>
       <c r="C8" s="147"/>
       <c r="D8" s="148"/>
@@ -9223,7 +9223,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B9" s="138"/>
       <c r="C9" s="147"/>
       <c r="D9" s="148"/>
@@ -9235,7 +9235,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="138"/>
       <c r="C10" s="147"/>
       <c r="D10" s="148"/>
@@ -9247,7 +9247,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B11" s="138"/>
       <c r="C11" s="147"/>
       <c r="D11" s="148"/>
@@ -9259,7 +9259,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B12" s="138"/>
       <c r="C12" s="147"/>
       <c r="D12" s="148"/>
@@ -9271,7 +9271,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B13" s="138"/>
       <c r="C13" s="139"/>
       <c r="D13" s="148"/>
@@ -9283,7 +9283,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B14" s="138"/>
       <c r="C14" s="147"/>
       <c r="D14" s="148"/>
@@ -9295,7 +9295,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B15" s="138"/>
       <c r="C15" s="147"/>
       <c r="D15" s="148"/>
@@ -9307,7 +9307,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B16" s="138"/>
       <c r="C16" s="147"/>
       <c r="D16" s="148"/>
@@ -9319,7 +9319,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B17" s="138"/>
       <c r="C17" s="147"/>
       <c r="D17" s="148"/>
@@ -9331,7 +9331,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B18" s="138"/>
       <c r="C18" s="147"/>
       <c r="D18" s="148"/>
@@ -9343,7 +9343,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B19" s="138"/>
       <c r="C19" s="147"/>
       <c r="D19" s="148"/>
@@ -9355,7 +9355,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B20" s="138"/>
       <c r="C20" s="147"/>
       <c r="D20" s="148"/>
@@ -9367,7 +9367,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="157"/>
       <c r="B21" s="138"/>
       <c r="C21" s="147"/>
@@ -9380,7 +9380,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B22" s="138"/>
       <c r="C22" s="147"/>
       <c r="D22" s="148"/>
@@ -9392,7 +9392,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B23" s="158"/>
       <c r="C23" s="158"/>
       <c r="D23" s="148"/>
@@ -9402,7 +9402,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B24" s="158"/>
       <c r="C24" s="158"/>
       <c r="D24" s="148"/>
@@ -9412,7 +9412,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B25" s="158"/>
       <c r="C25" s="158"/>
       <c r="D25" s="148"/>
@@ -9422,7 +9422,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B26" s="158"/>
       <c r="C26" s="158"/>
       <c r="D26" s="148"/>
@@ -9432,7 +9432,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B27" s="158"/>
       <c r="C27" s="158"/>
       <c r="D27" s="148"/>
@@ -9442,7 +9442,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="158"/>
       <c r="C28" s="158"/>
       <c r="D28" s="148"/>
@@ -9452,7 +9452,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="158"/>
       <c r="C29" s="158"/>
       <c r="D29" s="148"/>
@@ -9462,7 +9462,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B30" s="158"/>
       <c r="C30" s="158"/>
       <c r="D30" s="148"/>
@@ -9472,7 +9472,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B31" s="158"/>
       <c r="C31" s="158"/>
       <c r="D31" s="148"/>
@@ -9482,7 +9482,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B32" s="158"/>
       <c r="C32" s="158"/>
       <c r="D32" s="148"/>
@@ -9492,7 +9492,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B33" s="158"/>
       <c r="C33" s="158"/>
       <c r="D33" s="148"/>
@@ -9502,7 +9502,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B34" s="158"/>
       <c r="C34" s="158"/>
       <c r="D34" s="148"/>
@@ -9512,7 +9512,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B35" s="158"/>
       <c r="C35" s="158"/>
       <c r="D35" s="148"/>
@@ -9522,7 +9522,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B36" s="158"/>
       <c r="C36" s="158"/>
       <c r="D36" s="148"/>
@@ -9532,7 +9532,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B37" s="158"/>
       <c r="C37" s="158"/>
       <c r="D37" s="148"/>
@@ -9542,7 +9542,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B38" s="158"/>
       <c r="C38" s="158"/>
       <c r="D38" s="148"/>
@@ -9552,7 +9552,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" s="146" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A39" s="157"/>
       <c r="B39" s="158"/>
       <c r="C39" s="158"/>
@@ -9560,12 +9560,12 @@
       <c r="E39" s="148"/>
       <c r="F39" s="150"/>
     </row>
-    <row r="40" spans="1:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="159"/>
     </row>
-    <row r="41" spans="1:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" spans="1:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="43" spans="1:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B43" s="134" t="s">
         <v>88</v>
       </c>
@@ -9615,15 +9615,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
@@ -9644,57 +9635,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B7F6C1E041661428C0804F60FDF9579" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="269e77b516f09928499b1be999970057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17eb8759-252b-418d-a649-70aff91fc5df" xmlns:ns3="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720" xmlns:ns4="93977a9a-7c70-4c47-a38b-6f123b62dce6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41b65eea62d023978f15f5547645abd7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="17eb8759-252b-418d-a649-70aff91fc5df"/>
@@ -9915,15 +9865,57 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -9941,15 +9933,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5CD16F-1A82-4BAB-88E6-9D42833A2748}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9967,4 +9959,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Set a limit for the summary links
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/WATR_Template.xlsx
+++ b/AxeAccessibilityDriver/WATR_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DuongCh\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469A9BEC-54DC-408D-B86D-CBC5F72656B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AE03B4-CB4A-4D40-B72A-8763E57B95A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <definedName name="SuccessCriteria" localSheetId="1">#REF!</definedName>
     <definedName name="SuccessCriteria">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -4670,7 +4670,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A47" sqref="A47:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -5187,7 +5187,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:IR30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -6730,7 +6730,7 @@
   </sheetPr>
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
@@ -9053,7 +9053,7 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.4"/>
@@ -9615,6 +9615,56 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
@@ -9635,7 +9685,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9644,7 +9694,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B7F6C1E041661428C0804F60FDF9579" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="269e77b516f09928499b1be999970057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17eb8759-252b-418d-a649-70aff91fc5df" xmlns:ns3="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720" xmlns:ns4="93977a9a-7c70-4c47-a38b-6f123b62dce6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41b65eea62d023978f15f5547645abd7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="17eb8759-252b-418d-a649-70aff91fc5df"/>
@@ -9865,57 +9915,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -9933,7 +9941,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -9941,7 +9949,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5CD16F-1A82-4BAB-88E6-9D42833A2748}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9959,12 +9967,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>